<commit_message>
isqrt64 Improvements + fixed mulhi_u8
- Replaced the 64-bit square root with a implementation that is faster on older CPUs
- Added a new performance test file for sqrts
- Added a new performance test file for conversions
- Fixed an issue with odd elements in `mulHi_u8x16` performing low, rather than a high multiplication
</commit_message>
<xml_diff>
--- a/external/InstructionCost.xlsx
+++ b/external/InstructionCost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D242900-1BEB-44E0-A408-358A2E886345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF53295-1E52-4508-8779-FA97A451EB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
   </bookViews>
   <sheets>
     <sheet name="Emulated" sheetId="1" r:id="rId1"/>
@@ -196,6 +196,19 @@
     <author>Walter</author>
   </authors>
   <commentList>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{B74709FD-0C39-4300-BD12-5591651F5CB9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Even elements, not lower</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G8" authorId="0" shapeId="0" xr:uid="{1D344AC1-9880-462A-80BB-5254E9DC4DFC}">
       <text>
         <r>
@@ -259,6 +272,32 @@
             <family val="2"/>
           </rPr>
           <t>Using the float64 instruction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K62" authorId="0" shapeId="0" xr:uid="{3C464181-35DD-4443-B163-3225DCC98976}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Using int64</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K63" authorId="0" shapeId="0" xr:uid="{AC939DEA-E16F-4263-8B0B-BBD1DBF32E4E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Using int64</t>
         </r>
       </text>
     </comment>
@@ -332,7 +371,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="159">
   <si>
     <t>s8</t>
   </si>
@@ -514,9 +553,6 @@
     <t>horizontal sat. sub</t>
   </si>
   <si>
-    <t>insert to element</t>
-  </si>
-  <si>
     <t>full mul, add adjacent products</t>
   </si>
   <si>
@@ -809,6 +845,9 @@
   </si>
   <si>
     <t>ARITHMETIC</t>
+  </si>
+  <si>
+    <t>insert element (imm8)</t>
   </si>
 </sst>
 </file>
@@ -1235,20 +1274,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1727,9 +1766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60BA8C6-A487-451B-A2BD-8E39E20BCE51}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,7 +1810,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2188,21 +2227,21 @@
         <v>19</v>
       </c>
       <c r="B16" s="44">
-        <v>9</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45">
-        <v>1</v>
-      </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45">
+        <v>7</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42">
+        <v>1</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42">
         <v>8</v>
       </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45">
+      <c r="G16" s="42"/>
+      <c r="H16" s="42">
         <v>13</v>
       </c>
-      <c r="I16" s="46"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="1" t="s">
         <v>36</v>
       </c>
@@ -2282,7 +2321,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -2317,7 +2356,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" s="5">
         <v>43</v>
@@ -2349,15 +2388,15 @@
       <c r="K20" s="6">
         <v>1</v>
       </c>
-      <c r="L20" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
+      <c r="L20" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="1">
@@ -2377,13 +2416,13 @@
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1">
@@ -2405,13 +2444,13 @@
       <c r="K22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L22" s="42"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="1">
@@ -2429,9 +2468,9 @@
       <c r="I23" s="6"/>
       <c r="J23" s="1"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -2507,19 +2546,19 @@
       <c r="B26" s="44">
         <v>1</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45">
-        <v>1</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45">
-        <v>1</v>
-      </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45">
+      <c r="C26" s="42"/>
+      <c r="D26" s="42">
+        <v>1</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42">
+        <v>1</v>
+      </c>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42">
         <v>3</v>
       </c>
-      <c r="I26" s="46"/>
+      <c r="I26" s="43"/>
       <c r="J26" s="1">
         <v>1</v>
       </c>
@@ -2858,7 +2897,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>36</v>
@@ -2867,7 +2906,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" s="1">
         <v>3</v>
@@ -2893,7 +2932,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>36</v>
@@ -2928,7 +2967,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>36</v>
@@ -2963,7 +3002,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>36</v>
@@ -2998,20 +3037,34 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="L20:N23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K15 B16 D16 F16 H16 J16:K16 B17:K25 B26 D26 F26 H26 J26:K26 B27:K40">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"#"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:K40">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="5"/>
+        <cfvo type="num" val="18"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color rgb="FFE3F480"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:K25 B3:K15 B16 D16 F16 H16 J16:K16 B26 D26 F26 H26 J26:K26 B27:K40">
     <cfRule type="containsBlanks" dxfId="7" priority="12">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
@@ -3023,18 +3076,6 @@
         <cfvo type="max"/>
         <color rgb="FFFF0000"/>
         <color rgb="FF920000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:K40">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="5"/>
-        <cfvo type="num" val="18"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <color rgb="FFE3F480"/>
-        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3050,7 +3091,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,26 +3144,26 @@
         <v>10</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="50"/>
       <c r="D2" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2" s="51"/>
       <c r="J2" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L2" s="17"/>
       <c r="M2" s="31" t="s">
@@ -3134,26 +3175,26 @@
         <v>11</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="52"/>
       <c r="F3" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="52"/>
       <c r="H3" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="53"/>
       <c r="J3" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="31" t="s">
@@ -3165,30 +3206,30 @@
         <v>12</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="17"/>
       <c r="M4" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3196,123 +3237,123 @@
         <v>13</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="21"/>
       <c r="D6" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" s="17"/>
       <c r="M8" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
@@ -3323,7 +3364,7 @@
       <c r="K9" s="37"/>
       <c r="L9" s="17"/>
       <c r="M9" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3332,11 +3373,11 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -3346,7 +3387,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="17"/>
       <c r="M10" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3354,26 +3395,26 @@
         <v>15</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="18"/>
@@ -3395,14 +3436,14 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3410,34 +3451,34 @@
         <v>46</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="18"/>
       <c r="L13" s="17"/>
       <c r="M13" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3445,28 +3486,28 @@
         <v>47</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="18"/>
@@ -3480,30 +3521,30 @@
         <v>18</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="31" t="s">
@@ -3515,30 +3556,30 @@
         <v>17</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L16" s="17"/>
       <c r="M16" s="31" t="s">
@@ -3552,24 +3593,24 @@
       <c r="B17" s="55"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="47"/>
       <c r="F17" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
       <c r="I17" s="56"/>
       <c r="J17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -3579,24 +3620,24 @@
       <c r="B18" s="54"/>
       <c r="C18" s="52"/>
       <c r="D18" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
       <c r="I18" s="53"/>
       <c r="J18" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3606,7 +3647,7 @@
       <c r="B19" s="16"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -3617,7 +3658,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="17"/>
       <c r="M19" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3627,7 +3668,7 @@
       <c r="B20" s="24"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -3638,15 +3679,15 @@
       <c r="K20" s="25"/>
       <c r="L20" s="17"/>
       <c r="M20" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -3659,15 +3700,15 @@
       <c r="K21" s="18"/>
       <c r="L21" s="17"/>
       <c r="M21" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -3680,17 +3721,17 @@
       <c r="K22" s="18"/>
       <c r="L22" s="17"/>
       <c r="M22" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
@@ -3701,119 +3742,119 @@
       <c r="K23" s="18"/>
       <c r="L23" s="17"/>
       <c r="M23" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="18"/>
       <c r="L24" s="17"/>
       <c r="M24" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K25" s="26"/>
       <c r="L25" s="17"/>
       <c r="M25" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="17"/>
       <c r="M26" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
@@ -3824,19 +3865,19 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="23"/>
@@ -3847,14 +3888,14 @@
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
       <c r="J28" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -3891,30 +3932,30 @@
         <v>48</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="47"/>
       <c r="F31" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I31" s="56"/>
       <c r="J31" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3938,30 +3979,30 @@
         <v>49</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="62"/>
       <c r="D33" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="62"/>
       <c r="F33" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" s="62"/>
       <c r="H33" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I33" s="57"/>
       <c r="J33" s="61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K33" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L33" s="30"/>
       <c r="M33" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3980,7 +4021,7 @@
       <c r="K34" s="57"/>
       <c r="L34" s="30"/>
       <c r="M34" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -4046,334 +4087,334 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J39" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L39" s="17"/>
       <c r="M39" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L40" s="17"/>
       <c r="M40" s="48"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K41" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L41" s="17"/>
       <c r="M41" s="48"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K42" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L42" s="17"/>
       <c r="M42" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L43" s="17"/>
       <c r="M43" s="48"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L44" s="17"/>
       <c r="M44" s="48"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="J45" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L45" s="17"/>
       <c r="M45" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="16"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
       <c r="J46" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K46" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L46" s="17"/>
       <c r="M46" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
       <c r="F47" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L47" s="17"/>
       <c r="M47" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="16"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
       <c r="J48" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K48" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L48" s="17"/>
       <c r="M48" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -4410,7 +4451,7 @@
         <v>41</v>
       </c>
       <c r="B51" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C51" s="47"/>
       <c r="D51" s="47"/>
@@ -4420,10 +4461,10 @@
       <c r="H51" s="47"/>
       <c r="I51" s="56"/>
       <c r="J51" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L51" s="17"/>
       <c r="M51" s="31" t="s">
@@ -4435,7 +4476,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="52"/>
       <c r="D52" s="52"/>
@@ -4445,10 +4486,10 @@
       <c r="H52" s="52"/>
       <c r="I52" s="53"/>
       <c r="J52" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K52" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L52" s="17"/>
       <c r="M52" s="31" t="s">
@@ -4460,7 +4501,7 @@
         <v>54</v>
       </c>
       <c r="B53" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C53" s="52"/>
       <c r="D53" s="52"/>
@@ -4470,10 +4511,10 @@
       <c r="H53" s="52"/>
       <c r="I53" s="53"/>
       <c r="J53" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K53" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L53" s="17"/>
       <c r="M53" s="31" t="s">
@@ -4482,10 +4523,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="52"/>
       <c r="D54" s="52"/>
@@ -4495,115 +4536,115 @@
       <c r="H54" s="52"/>
       <c r="I54" s="53"/>
       <c r="J54" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K54" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L54" s="17"/>
       <c r="M54" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="54"/>
       <c r="C55" s="52"/>
       <c r="D55" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E55" s="52"/>
       <c r="F55" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G55" s="52"/>
       <c r="H55" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I55" s="53"/>
       <c r="J55" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K55" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L55" s="17"/>
       <c r="M55" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J56" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K56" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L56" s="17"/>
       <c r="M56" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="24"/>
       <c r="C57" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H57" s="23"/>
       <c r="I57" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J57" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L57" s="17"/>
       <c r="M57" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -4642,7 +4683,7 @@
       <c r="B60" s="55"/>
       <c r="C60" s="47"/>
       <c r="D60" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E60" s="47"/>
       <c r="F60" s="47"/>
@@ -4650,17 +4691,17 @@
       <c r="H60" s="47"/>
       <c r="I60" s="56"/>
       <c r="J60" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K60" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L60" s="17"/>
       <c r="M60" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N60" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -4668,97 +4709,101 @@
         <v>45</v>
       </c>
       <c r="B61" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C61" s="52"/>
       <c r="D61" s="52"/>
       <c r="E61" s="52"/>
       <c r="F61" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G61" s="52"/>
       <c r="H61" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I61" s="53"/>
       <c r="J61" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K61" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L61" s="17"/>
       <c r="M61" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" s="52"/>
       <c r="D62" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E62" s="52"/>
       <c r="F62" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G62" s="52"/>
       <c r="H62" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I62" s="53"/>
       <c r="J62" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="K62" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="K62" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="L62" s="17"/>
       <c r="M62" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="B63" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" s="52"/>
       <c r="D63" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E63" s="52"/>
       <c r="F63" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G63" s="52"/>
       <c r="H63" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I63" s="53"/>
       <c r="J63" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="K63" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="K63" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="L63" s="17"/>
       <c r="M63" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="16"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
       <c r="E64" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
@@ -4768,48 +4813,48 @@
       <c r="K64" s="18"/>
       <c r="L64" s="17"/>
       <c r="M64" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B65" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="52"/>
       <c r="D65" s="52"/>
       <c r="E65" s="52"/>
       <c r="F65" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G65" s="52"/>
       <c r="H65" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I65" s="53"/>
       <c r="J65" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K65" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L65" s="17"/>
       <c r="M65" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B66" s="55"/>
       <c r="C66" s="47"/>
       <c r="D66" s="47"/>
       <c r="E66" s="47"/>
       <c r="F66" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G66" s="47"/>
       <c r="H66" s="47"/>
@@ -4818,15 +4863,15 @@
       <c r="K66" s="56"/>
       <c r="L66" s="17"/>
       <c r="M66" s="48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="17"/>
@@ -4842,12 +4887,12 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B68" s="54"/>
       <c r="C68" s="52"/>
       <c r="D68" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E68" s="52"/>
       <c r="F68" s="52"/>
@@ -4858,17 +4903,17 @@
       <c r="K68" s="18"/>
       <c r="L68" s="17"/>
       <c r="M68" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B69" s="54"/>
       <c r="C69" s="52"/>
       <c r="D69" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E69" s="52"/>
       <c r="F69" s="52"/>
@@ -4879,96 +4924,96 @@
       <c r="K69" s="18"/>
       <c r="L69" s="17"/>
       <c r="M69" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="58"/>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
       <c r="E70" s="59"/>
       <c r="F70" s="59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G70" s="59"/>
       <c r="H70" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I70" s="60"/>
       <c r="J70" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K70" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L70" s="17"/>
       <c r="M70" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="52"/>
       <c r="D71" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E71" s="52"/>
       <c r="F71" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G71" s="52"/>
       <c r="H71" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I71" s="53"/>
       <c r="J71" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K71" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L71" s="17"/>
       <c r="M71" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C72" s="64"/>
       <c r="D72" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E72" s="64"/>
       <c r="F72" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G72" s="64"/>
       <c r="H72" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I72" s="65"/>
       <c r="J72" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K72" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L72" s="17"/>
       <c r="M72" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5166,7 +5211,7 @@
           <x14:formula1>
             <xm:f>enums!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G5 G61:I65 G67:L72 E61:F72 B2:F20 B21:D72 H2:L20 J21:L65 E21:I59 G7:G20</xm:sqref>
+          <xm:sqref>G2:G5 G61:I65 G67:L72 E61:F72 B2:F20 B21:D72 H2:L20 G7:G20 E21:I59 J21:L65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5189,47 +5234,47 @@
   <sheetData>
     <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved `udiv32/umod32` + minor changes
- Replaced shift with a cast in the `_getMSB_i16` function, which sometimes saves on an instruction
- Unsigned 32-bit div/mod: Replaced calls to `_convert_f64x2_u32x4` with signed instruction + correction as the only case where it can overflow is div by one (20% performance increase!)
- Added reverse functions for individually setting the divisors for the division by a constant methods (`_getDivMagic_setr`)
- Added additional information to the performance excel documents, which now includes more micro-architectures
- Updated the performance matrix to reflect these changes
</commit_message>
<xml_diff>
--- a/external/InstructionCost.xlsx
+++ b/external/InstructionCost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF53295-1E52-4508-8779-FA97A451EB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C8295-E46D-4733-96E9-C2FCFBF31BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
   </bookViews>
   <sheets>
     <sheet name="Emulated" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D60" authorId="0" shapeId="0" xr:uid="{5DE93A55-7E8C-418C-B9F4-313156BA5399}">
+    <comment ref="D64" authorId="0" shapeId="0" xr:uid="{5DE93A55-7E8C-418C-B9F4-313156BA5399}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F61" authorId="0" shapeId="0" xr:uid="{533B915A-C1A3-4834-A6EB-5D291566E311}">
+    <comment ref="F65" authorId="0" shapeId="0" xr:uid="{533B915A-C1A3-4834-A6EB-5D291566E311}">
       <text>
         <r>
           <rPr>
@@ -262,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H61" authorId="0" shapeId="0" xr:uid="{76A5A45D-4B8B-476A-81B1-DEDF8978038D}">
+    <comment ref="H65" authorId="0" shapeId="0" xr:uid="{76A5A45D-4B8B-476A-81B1-DEDF8978038D}">
       <text>
         <r>
           <rPr>
@@ -275,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K62" authorId="0" shapeId="0" xr:uid="{3C464181-35DD-4443-B163-3225DCC98976}">
+    <comment ref="K66" authorId="0" shapeId="0" xr:uid="{3C464181-35DD-4443-B163-3225DCC98976}">
       <text>
         <r>
           <rPr>
@@ -288,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K63" authorId="0" shapeId="0" xr:uid="{AC939DEA-E16F-4263-8B0B-BBD1DBF32E4E}">
+    <comment ref="K67" authorId="0" shapeId="0" xr:uid="{AC939DEA-E16F-4263-8B0B-BBD1DBF32E4E}">
       <text>
         <r>
           <rPr>
@@ -301,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F65" authorId="0" shapeId="0" xr:uid="{42434C9D-1B3C-4F9C-85C1-2BB6E085EDEE}">
+    <comment ref="F69" authorId="0" shapeId="0" xr:uid="{42434C9D-1B3C-4F9C-85C1-2BB6E085EDEE}">
       <text>
         <r>
           <rPr>
@@ -314,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H65" authorId="0" shapeId="0" xr:uid="{7A8C1B2F-7298-4403-89F3-422B0334CF22}">
+    <comment ref="H69" authorId="0" shapeId="0" xr:uid="{7A8C1B2F-7298-4403-89F3-422B0334CF22}">
       <text>
         <r>
           <rPr>
@@ -327,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F66" authorId="0" shapeId="0" xr:uid="{6B421FFF-86EF-4663-B432-C8A9B0973E83}">
+    <comment ref="F70" authorId="0" shapeId="0" xr:uid="{6B421FFF-86EF-4663-B432-C8A9B0973E83}">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F70" authorId="0" shapeId="0" xr:uid="{F1214490-6D68-48C2-9C1E-98CBDB71F01B}">
+    <comment ref="F74" authorId="0" shapeId="0" xr:uid="{F1214490-6D68-48C2-9C1E-98CBDB71F01B}">
       <text>
         <r>
           <rPr>
@@ -353,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H70" authorId="0" shapeId="0" xr:uid="{F0967501-55ED-43B2-9DB8-BAF95370661B}">
+    <comment ref="H74" authorId="0" shapeId="0" xr:uid="{F0967501-55ED-43B2-9DB8-BAF95370661B}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="175">
   <si>
     <t>s8</t>
   </si>
@@ -622,21 +622,12 @@
     <t>SSE4.2</t>
   </si>
   <si>
-    <t>SSE Version</t>
-  </si>
-  <si>
     <t>SSE</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>shift left</t>
-  </si>
-  <si>
-    <t>sign right shift</t>
-  </si>
-  <si>
     <t>Dot product</t>
   </si>
   <si>
@@ -667,9 +658,6 @@
     <t>approx. reciprocal</t>
   </si>
   <si>
-    <t>logical shift right</t>
-  </si>
-  <si>
     <t>arg1 but sign set to arg2 (0=0)</t>
   </si>
   <si>
@@ -760,9 +748,6 @@
     <t>cvt##_pd</t>
   </si>
   <si>
-    <t>cvtp[s,d]_epi32</t>
-  </si>
-  <si>
     <t>sll</t>
   </si>
   <si>
@@ -848,13 +833,76 @@
   </si>
   <si>
     <t>insert element (imm8)</t>
+  </si>
+  <si>
+    <t>AVX2</t>
+  </si>
+  <si>
+    <t>logical shift right (vector)</t>
+  </si>
+  <si>
+    <t>sign right shift (scalar)</t>
+  </si>
+  <si>
+    <t>logical shift right (scalar)</t>
+  </si>
+  <si>
+    <t>shift left (vector)</t>
+  </si>
+  <si>
+    <t>shift left (scalar)</t>
+  </si>
+  <si>
+    <t>sllv</t>
+  </si>
+  <si>
+    <t>srlv</t>
+  </si>
+  <si>
+    <t>srav</t>
+  </si>
+  <si>
+    <t>sign right shift (vector)</t>
+  </si>
+  <si>
+    <t>cvt##_epi32</t>
+  </si>
+  <si>
+    <t>512ER</t>
+  </si>
+  <si>
+    <t>512POPCNT</t>
+  </si>
+  <si>
+    <t>512VBMI2+</t>
+  </si>
+  <si>
+    <t>512DQ/BW</t>
+  </si>
+  <si>
+    <t>512F</t>
+  </si>
+  <si>
+    <t>+VL</t>
+  </si>
+  <si>
+    <t>+BITALG, VPCLMUL., GFNI, VAES</t>
+  </si>
+  <si>
+    <t>## TODO: AVX512 to u32, i64, u64</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Includes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,6 +966,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1155,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,44 +1250,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1252,18 +1275,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1274,6 +1285,61 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,76 +1347,97 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.34998626667073579"/>
@@ -1766,9 +1853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60BA8C6-A487-451B-A2BD-8E39E20BCE51}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,41 +1863,41 @@
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2229,19 +2316,19 @@
       <c r="B16" s="44">
         <v>7</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42">
-        <v>1</v>
-      </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42">
+      <c r="C16" s="45"/>
+      <c r="D16" s="45">
+        <v>1</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45">
         <v>8</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42">
+      <c r="G16" s="45"/>
+      <c r="H16" s="45">
         <v>13</v>
       </c>
-      <c r="I16" s="43"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="1" t="s">
         <v>36</v>
       </c>
@@ -2356,7 +2443,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B20" s="5">
         <v>43</v>
@@ -2374,12 +2461,12 @@
         <v>11</v>
       </c>
       <c r="G20" s="1">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H20" s="1">
         <v>14</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="22">
         <v>14</v>
       </c>
       <c r="J20" s="1">
@@ -2388,15 +2475,15 @@
       <c r="K20" s="6">
         <v>1</v>
       </c>
-      <c r="L20" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
+      <c r="L20" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="1">
@@ -2408,21 +2495,21 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="38">
+      <c r="I21" s="22">
         <v>14</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1">
@@ -2444,13 +2531,13 @@
       <c r="K22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L22" s="45"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="1">
@@ -2468,9 +2555,9 @@
       <c r="I23" s="6"/>
       <c r="J23" s="1"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -2546,19 +2633,19 @@
       <c r="B26" s="44">
         <v>1</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42">
-        <v>1</v>
-      </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42">
-        <v>1</v>
-      </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42">
+      <c r="C26" s="45"/>
+      <c r="D26" s="45">
+        <v>1</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45">
+        <v>1</v>
+      </c>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45">
         <v>3</v>
       </c>
-      <c r="I26" s="43"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="1">
         <v>1</v>
       </c>
@@ -2967,7 +3054,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>36</v>
@@ -2978,7 +3065,7 @@
       <c r="D39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="39" t="s">
+      <c r="E39" s="23" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="1">
@@ -3002,7 +3089,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>36</v>
@@ -3037,6 +3124,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L20:N23"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
@@ -3045,10 +3133,9 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="L20:N23"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K15 B16 D16 F16 H16 J16:K16 B17:K25 B26 D26 F26 H26 J26:K26 B27:K40">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3065,7 +3152,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K25 B3:K15 B16 D16 F16 H16 J16:K16 B26 D26 F26 H26 J26:K26 B27:K40">
-    <cfRule type="containsBlanks" dxfId="7" priority="12">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3087,11 +3174,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB52227-ACC2-4A13-BAC7-C7465281EE66}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N72" sqref="N72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,74 +3186,74 @@
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="2.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="31" customWidth="1"/>
-    <col min="14" max="14" width="68.7109375" style="32" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="68.7109375" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="28"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="31" t="s">
+      <c r="B2" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="57"/>
+      <c r="J2" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3174,7 +3261,7 @@
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="51" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="52"/>
@@ -3190,14 +3277,14 @@
         <v>78</v>
       </c>
       <c r="I3" s="53"/>
-      <c r="J3" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="31" t="s">
+      <c r="J3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3205,221 +3292,225 @@
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="31" t="s">
-        <v>101</v>
+      <c r="B4" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="31" t="s">
-        <v>100</v>
+      <c r="B5" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="31" t="s">
-        <v>102</v>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="50"/>
+      <c r="J6" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="31" t="s">
-        <v>103</v>
+      <c r="B7" s="27"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="31" t="s">
-        <v>104</v>
+      <c r="G8" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="19" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="31" t="s">
-        <v>112</v>
+      <c r="D9" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="31" t="s">
-        <v>105</v>
+      <c r="B10" s="27"/>
+      <c r="C10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="31" t="s">
+      <c r="G11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3427,92 +3518,92 @@
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="31" t="s">
-        <v>106</v>
+      <c r="L12" s="14"/>
+      <c r="M12" s="19" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="31" t="s">
-        <v>107</v>
+      <c r="B13" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="19" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="31" t="s">
+      <c r="B14" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="27"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3520,34 +3611,38 @@
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="C15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="31" t="s">
+      <c r="H15" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3555,34 +3650,38 @@
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="C16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="31" t="s">
+      <c r="H16" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3590,34 +3689,34 @@
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47" t="s">
+      <c r="E17" s="49"/>
+      <c r="F17" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="22" t="s">
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="31" t="s">
-        <v>108</v>
+      <c r="L17" s="14"/>
+      <c r="M17" s="19" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="54"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="52"/>
       <c r="D18" s="52" t="s">
         <v>80</v>
@@ -3629,878 +3728,923 @@
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
       <c r="I18" s="53"/>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="31" t="s">
-        <v>109</v>
+      <c r="L18" s="14"/>
+      <c r="M18" s="19" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="31" t="s">
-        <v>110</v>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="19" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="31" t="s">
-        <v>111</v>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="19" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="31" t="s">
-        <v>113</v>
+      <c r="B21" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="31" t="s">
-        <v>114</v>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="31" t="s">
-        <v>115</v>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="17" t="s">
+      <c r="E24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="31" t="s">
-        <v>116</v>
+      <c r="G24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="31" t="s">
-        <v>117</v>
+        <v>94</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="35"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="19" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="31" t="s">
-        <v>118</v>
+      <c r="B26" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="L26" s="14"/>
+      <c r="M26" s="19" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="31" t="s">
-        <v>119</v>
+      <c r="B27" s="27"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" s="14"/>
+      <c r="M27" s="19" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="K28" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="31" t="s">
-        <v>120</v>
+      <c r="L28" s="14"/>
+      <c r="M28" s="19" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="17"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="17"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47" t="s">
+      <c r="B31" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="56"/>
-      <c r="J31" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="K31" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="17"/>
-      <c r="M31" s="31" t="s">
-        <v>121</v>
+      <c r="I31" s="50"/>
+      <c r="J31" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" s="14"/>
+      <c r="M31" s="19" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="17"/>
+      <c r="B32" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="I32" s="53"/>
+      <c r="J32" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62" t="s">
+      <c r="B33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="H33" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I33" s="57"/>
-      <c r="J33" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="K33" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="L33" s="30"/>
-      <c r="M33" s="31" t="s">
-        <v>122</v>
+      <c r="I33" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="J33" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="18"/>
+      <c r="M33" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="31" t="s">
-        <v>123</v>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="19" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="17"/>
+      <c r="B35" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="I35" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="J35" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="L35" s="14"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="17"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="17"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="17"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="21" t="s">
+      <c r="D39" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="F39" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="21" t="s">
+      <c r="F39" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="H39" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="J39" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K39" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="L39" s="17"/>
-      <c r="M39" s="48" t="s">
-        <v>124</v>
+      <c r="H39" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="K39" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L39" s="14"/>
+      <c r="M39" s="54" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" s="17" t="s">
+      <c r="D40" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L40" s="17"/>
-      <c r="M40" s="48"/>
+      <c r="F40" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K40" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L40" s="14"/>
+      <c r="M40" s="54"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K41" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="48"/>
+      <c r="D41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J41" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K41" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="14"/>
+      <c r="M41" s="54"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="17" t="s">
+      <c r="C42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="17" t="s">
+      <c r="E42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L42" s="17"/>
-      <c r="M42" s="48" t="s">
-        <v>125</v>
+      <c r="G42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J42" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K42" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L42" s="14"/>
+      <c r="M42" s="54" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="17" t="s">
+      <c r="C43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="48"/>
+      <c r="E43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J43" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L43" s="14"/>
+      <c r="M43" s="54"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L44" s="17"/>
-      <c r="M44" s="48"/>
+      <c r="C44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J44" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L44" s="14"/>
+      <c r="M44" s="54"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G45" s="17" t="s">
+      <c r="B45" s="27"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L45" s="17"/>
-      <c r="M45" s="31" t="s">
-        <v>126</v>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K45" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L45" s="14"/>
+      <c r="M45" s="19" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K46" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L46" s="17"/>
-      <c r="M46" s="31" t="s">
-        <v>127</v>
+      <c r="B46" s="27"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K46" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L46" s="14"/>
+      <c r="M46" s="19" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="K47" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L47" s="17"/>
-      <c r="M47" s="31" t="s">
-        <v>128</v>
+      <c r="B47" s="27"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J47" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K47" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L47" s="14"/>
+      <c r="M47" s="19" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="K48" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L48" s="17"/>
-      <c r="M48" s="31" t="s">
-        <v>129</v>
+      <c r="B48" s="27"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K48" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L48" s="14"/>
+      <c r="M48" s="19" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="54"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="54"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="17"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A49" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" s="27"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="14"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="51"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="14"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="60"/>
-      <c r="L50" s="17"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="K51" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="L51" s="17"/>
-      <c r="M51" s="31" t="s">
-        <v>41</v>
-      </c>
+      <c r="B51" s="59"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="59"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="14"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K52" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L52" s="17"/>
-      <c r="M52" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B52" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K52" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L52" s="14"/>
+      <c r="M52" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="51" t="s">
         <v>78</v>
       </c>
       <c r="C53" s="52"/>
@@ -4510,22 +4654,22 @@
       <c r="G53" s="52"/>
       <c r="H53" s="52"/>
       <c r="I53" s="53"/>
-      <c r="J53" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K53" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L53" s="17"/>
-      <c r="M53" s="31" t="s">
-        <v>54</v>
+      <c r="J53" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K53" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L53" s="14"/>
+      <c r="M53" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="51" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="52"/>
@@ -4535,495 +4679,606 @@
       <c r="G54" s="52"/>
       <c r="H54" s="52"/>
       <c r="I54" s="53"/>
-      <c r="J54" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L54" s="17"/>
-      <c r="M54" s="31" t="s">
-        <v>74</v>
+      <c r="J54" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K54" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L54" s="14"/>
+      <c r="M54" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="54"/>
+        <v>74</v>
+      </c>
+      <c r="B55" s="51" t="s">
+        <v>78</v>
+      </c>
       <c r="C55" s="52"/>
-      <c r="D55" s="52" t="s">
-        <v>78</v>
-      </c>
+      <c r="D55" s="52"/>
       <c r="E55" s="52"/>
-      <c r="F55" s="52" t="s">
-        <v>78</v>
-      </c>
+      <c r="F55" s="52"/>
       <c r="G55" s="52"/>
-      <c r="H55" s="52" t="s">
-        <v>78</v>
-      </c>
+      <c r="H55" s="52"/>
       <c r="I55" s="53"/>
-      <c r="J55" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K55" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L55" s="17"/>
-      <c r="M55" s="31" t="s">
-        <v>130</v>
+      <c r="J55" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K55" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L55" s="14"/>
+      <c r="M55" s="19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K56" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="31" t="s">
-        <v>131</v>
+        <v>159</v>
+      </c>
+      <c r="B56" s="51"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" s="53"/>
+      <c r="J56" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K56" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L56" s="14"/>
+      <c r="M56" s="19" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F57" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="G57" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J57" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="K57" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="L57" s="17"/>
-      <c r="M57" s="31" t="s">
-        <v>132</v>
+        <v>158</v>
+      </c>
+      <c r="B57" s="51"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="I57" s="53"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="19" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="55"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="17"/>
-    </row>
-    <row r="59" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="17"/>
+      <c r="A58" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H58" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J58" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="K58" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="L58" s="14"/>
+      <c r="M58" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="51"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F59" s="52"/>
+      <c r="G59" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H59" s="52"/>
+      <c r="I59" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="J59" s="51"/>
+      <c r="K59" s="53"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="19" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="55"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="K60" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="L60" s="17"/>
-      <c r="M60" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="N60" s="33" t="s">
-        <v>147</v>
+        <v>156</v>
+      </c>
+      <c r="B60" s="27"/>
+      <c r="C60" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G60" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I60" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="J60" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="K60" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="L60" s="13"/>
+      <c r="M60" s="19" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="I61" s="53"/>
-      <c r="J61" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="K61" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L61" s="17"/>
-      <c r="M61" s="31" t="s">
-        <v>134</v>
+        <v>163</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="60"/>
+      <c r="F61" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G61" s="60"/>
+      <c r="H61" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I61" s="61"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="19" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B62" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="I62" s="53"/>
-      <c r="J62" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K62" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L62" s="17"/>
-      <c r="M62" s="31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B63" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="I63" s="53"/>
-      <c r="J63" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K63" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L63" s="17"/>
-      <c r="M63" s="31" t="s">
-        <v>136</v>
-      </c>
+      <c r="B62" s="58"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="58"/>
+      <c r="K62" s="50"/>
+      <c r="L62" s="14"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="59"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="61"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="61"/>
+      <c r="L63" s="14"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" s="58"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="31" t="s">
-        <v>137</v>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K64" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="L64" s="14"/>
+      <c r="M64" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="N64" s="21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B65" s="54" t="s">
-        <v>78</v>
+        <v>45</v>
+      </c>
+      <c r="B65" s="51" t="s">
+        <v>81</v>
       </c>
       <c r="C65" s="52"/>
       <c r="D65" s="52"/>
       <c r="E65" s="52"/>
       <c r="F65" s="52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G65" s="52"/>
       <c r="H65" s="52" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I65" s="53"/>
-      <c r="J65" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K65" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L65" s="17"/>
-      <c r="M65" s="31" t="s">
-        <v>138</v>
+      <c r="J65" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K65" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L65" s="14"/>
+      <c r="M65" s="19" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="G66" s="47"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47"/>
-      <c r="J66" s="47"/>
-      <c r="K66" s="56"/>
-      <c r="L66" s="17"/>
-      <c r="M66" s="48" t="s">
-        <v>139</v>
+        <v>86</v>
+      </c>
+      <c r="B66" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="52"/>
+      <c r="F66" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="I66" s="53"/>
+      <c r="J66" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K66" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L66" s="14"/>
+      <c r="M66" s="19" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="48"/>
+        <v>153</v>
+      </c>
+      <c r="B67" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="52"/>
+      <c r="F67" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G67" s="52"/>
+      <c r="H67" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="I67" s="53"/>
+      <c r="J67" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K67" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L67" s="14"/>
+      <c r="M67" s="19" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B68" s="54"/>
-      <c r="C68" s="52"/>
-      <c r="D68" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
-      <c r="H68" s="52"/>
-      <c r="I68" s="53"/>
-      <c r="J68" s="16"/>
-      <c r="K68" s="18"/>
-      <c r="L68" s="17"/>
-      <c r="M68" s="31" t="s">
-        <v>140</v>
+        <v>61</v>
+      </c>
+      <c r="B68" s="27"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="27"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B69" s="54"/>
+        <v>93</v>
+      </c>
+      <c r="B69" s="51" t="s">
+        <v>78</v>
+      </c>
       <c r="C69" s="52"/>
       <c r="D69" s="52" t="s">
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="E69" s="52"/>
-      <c r="F69" s="52"/>
+      <c r="F69" s="52" t="s">
+        <v>83</v>
+      </c>
       <c r="G69" s="52"/>
-      <c r="H69" s="52"/>
+      <c r="H69" s="52" t="s">
+        <v>78</v>
+      </c>
       <c r="I69" s="53"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="31" t="s">
-        <v>141</v>
+      <c r="J69" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K69" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L69" s="14"/>
+      <c r="M69" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="B70" s="58"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="G70" s="59"/>
-      <c r="H70" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="I70" s="60"/>
-      <c r="J70" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K70" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="L70" s="17"/>
-      <c r="M70" s="31" t="s">
-        <v>139</v>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71" s="54" t="s">
-        <v>78</v>
+        <v>140</v>
+      </c>
+      <c r="B71" s="51" t="s">
+        <v>80</v>
       </c>
       <c r="C71" s="52"/>
       <c r="D71" s="52" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="E71" s="52"/>
-      <c r="F71" s="52" t="s">
-        <v>78</v>
-      </c>
+      <c r="F71" s="52"/>
       <c r="G71" s="52"/>
-      <c r="H71" s="52" t="s">
-        <v>78</v>
-      </c>
+      <c r="H71" s="52"/>
       <c r="I71" s="53"/>
-      <c r="J71" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K71" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L71" s="17"/>
-      <c r="M71" s="31" t="s">
-        <v>143</v>
-      </c>
+      <c r="J71" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="K71" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L71" s="14"/>
+      <c r="M71" s="54"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="51"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="52"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="26"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="51"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="59"/>
+      <c r="C74" s="60"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="60"/>
+      <c r="F74" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" s="60"/>
+      <c r="H74" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I74" s="61"/>
+      <c r="J74" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K74" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L74" s="14"/>
+      <c r="M74" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" s="52"/>
+      <c r="D75" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="52"/>
+      <c r="F75" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="52"/>
+      <c r="H75" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="I75" s="53"/>
+      <c r="J75" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K75" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L75" s="14"/>
+      <c r="M75" s="19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="G72" s="64"/>
-      <c r="H72" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="I72" s="65"/>
-      <c r="J72" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="K72" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="L72" s="17"/>
-      <c r="M72" s="31" t="s">
-        <v>142</v>
+      <c r="B76" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="63"/>
+      <c r="F76" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="I76" s="64"/>
+      <c r="J76" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K76" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="L76" s="14"/>
+      <c r="M76" s="19" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="127">
+    <mergeCell ref="B58:B59"/>
     <mergeCell ref="B29:I30"/>
     <mergeCell ref="J29:K30"/>
     <mergeCell ref="B37:I38"/>
     <mergeCell ref="J37:K38"/>
-    <mergeCell ref="B49:I50"/>
-    <mergeCell ref="J49:K50"/>
+    <mergeCell ref="B50:I51"/>
+    <mergeCell ref="J50:K51"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="D18:E18"/>
@@ -5040,52 +5295,97 @@
     <mergeCell ref="K35:K36"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="K33:K34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="B67:C67"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="F72:G72"/>
     <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H70:I70"/>
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="F69:G69"/>
     <mergeCell ref="H69:I69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:K70"/>
+    <mergeCell ref="J62:K63"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D64:I64"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B62:I63"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="H71:I71"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:K66"/>
-    <mergeCell ref="J58:K59"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="D60:I60"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B58:I59"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="M39:M41"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="M70:M71"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="E35:E36"/>
@@ -5096,30 +5396,9 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="M66:M67"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5201,17 +5480,60 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B2:B3 D2:D3 F2:F3 H2:H3 J2:L3 B4:L5 B6:D6 F6 H6:L6 B7:L16 M8:M9 B17:B18 D17:D18 F17:F18 H17:H18 J17:L18 B19:L28 B29 J29 B31 D31 F31 H31 J31:L31 B32:L33 B35:L35 B37 J37 B39:L48 B49 J49 J51:L57 B51:B58 D55 F55:F56 H55:H56 B56:L57 J58 N60 B60:B63 D60:D63 J60:L63 F61:F63 H61:H63 B64:L64 H65 J65:L65 B65:B72 D65:D72 F65:F72 H67:H72 J67:L72</xm:sqref>
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{7B6DFD13-FCEF-4884-963C-159C415F8201}">
+            <xm:f>enums!$A$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{911188AA-777A-48C0-BB67-B7A7FD7A956D}">
+            <xm:f>enums!$A$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="beginsWith" priority="10" operator="beginsWith" id="{3DE8F479-383F-4D18-8260-B3B4D4C38BB7}">
+            <xm:f>LEFT(B2,LEN("512"))="512"</xm:f>
+            <xm:f>"512"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B2:B3 D2:D3 F2:F3 H2:H3 J2:L3 B4:L5 B6:D6 F6 H6 J6:L6 B7:L16 M8:M9 B17:B18 D17:D18 F17:F18 H17:H18 J17:L18 B19:L28 B29 J29 B31:B32 D31:D32 F31:F32 H31:H32 J31:L32 B33:L33 B35:L35 B37 J37 B39:L49 B50 J50 B52:B58 J52:L58 D56:D57 F56:F58 H56:H58 B58:L58 C59 E59 G59 I59 L59 B60:L60 B60:B62 D61 F61 H61 L61 J62 N64 B64:B67 D64:D67 J64:L67 F65:F67 H65:H67 B68:L68 H69 J69:L69 B69:B76 D69:D76 F69:F76 H71:H76 J71:L76</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F11E4542-0239-4C63-8AE0-1B546B3FC625}">
           <x14:formula1>
             <xm:f>enums!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G5 G61:I65 G67:L72 E61:F72 B2:F20 B21:D72 H2:L20 G7:G20 E21:I59 J21:L65</xm:sqref>
+          <xm:sqref>L71:L76 L2:L69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{DEBE69DA-103A-4DD0-BF69-DA4523CE4777}">
+          <x14:formula1>
+            <xm:f>enums!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F76 I7:I31 C2:C31 G72:G76 D2:D76 E2:E31 H2:H76 E72:E76 G2:G31 C72:C76 J2:K76 B60:B76 B2:B58 I2:I5 C33:C70 E33:E70 G33:G70 I33:I70 I72:I76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5221,60 +5543,100 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42270057-09F5-4DBC-B29A-71117FFFAFC1}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added variable shift & shuffle
- Added variable shuffle by vector for all element sizes
- Added variable left and right shift for all element sizes
- Added performance testes measuring a bunch of different shift and shuffle methods
- Added a excel file documenting the performance of those test on different computers/compilers
- Replaced the multiple almost identical functions for measuring conversion performance with a function generator

I plan on adding images of the excel file in the repository to make it more accessible. Also, I will update the wiki to include the new functions.
</commit_message>
<xml_diff>
--- a/external/InstructionCost.xlsx
+++ b/external/InstructionCost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C8295-E46D-4733-96E9-C2FCFBF31BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB0BDD-C2F9-4C41-B3AE-CAA690E996FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
   </bookViews>
   <sheets>
     <sheet name="Emulated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>Walter</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{55744591-C7FE-4654-B0E5-44537780EB51}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{55744591-C7FE-4654-B0E5-44537780EB51}">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{B0E9962C-F9B2-487F-8C5D-89230F3C0E4F}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{B0E9962C-F9B2-487F-8C5D-89230F3C0E4F}">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{CF63EA4B-17A8-4913-BE1D-DCE94EFDCE67}">
+    <comment ref="H21" authorId="0" shapeId="0" xr:uid="{CF63EA4B-17A8-4913-BE1D-DCE94EFDCE67}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{75A48089-3299-4780-8CB1-1D19939C8FF2}">
+    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{75A48089-3299-4780-8CB1-1D19939C8FF2}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{4605C02D-84FE-4C92-9A1B-5A8AD2E120C6}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{4605C02D-84FE-4C92-9A1B-5A8AD2E120C6}">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{D60473DB-86FB-4ABE-8FEE-89171537639D}">
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{D60473DB-86FB-4ABE-8FEE-89171537639D}">
       <text>
         <r>
           <rPr>
@@ -121,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{76B590EA-B4FC-4066-A7E3-4035C54ABC67}">
+    <comment ref="I23" authorId="0" shapeId="0" xr:uid="{76B590EA-B4FC-4066-A7E3-4035C54ABC67}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{FA7B4D9A-7D0D-4E6D-A3DE-5EDDE33F39FD}">
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{FA7B4D9A-7D0D-4E6D-A3DE-5EDDE33F39FD}">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{7347B22F-CE06-4A5E-8E06-1BFFE8299DF8}">
+    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{7347B22F-CE06-4A5E-8E06-1BFFE8299DF8}">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I35" authorId="0" shapeId="0" xr:uid="{0884A547-266D-4F79-9614-C51EDCD73B95}">
+    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{0884A547-266D-4F79-9614-C51EDCD73B95}">
       <text>
         <r>
           <rPr>
@@ -173,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0" shapeId="0" xr:uid="{FC74B33C-5D5E-4701-99E4-77FA4F8831B8}">
+    <comment ref="D39" authorId="0" shapeId="0" xr:uid="{FC74B33C-5D5E-4701-99E4-77FA4F8831B8}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="178">
   <si>
     <t>s8</t>
   </si>
@@ -896,6 +896,15 @@
   </si>
   <si>
     <t>Includes</t>
+  </si>
+  <si>
+    <t>shift left by vector</t>
+  </si>
+  <si>
+    <t>shift right by vector</t>
+  </si>
+  <si>
+    <t>shuffle by vector</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1337,6 +1346,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1346,11 +1367,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1358,7 +1379,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1367,43 +1394,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1851,11 +1863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60BA8C6-A487-451B-A2BD-8E39E20BCE51}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,229 +2188,213 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="B11" s="48">
+        <v>27</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49">
+        <v>17</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49">
+        <v>12</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49">
+        <v>6</v>
+      </c>
+      <c r="I11" s="50"/>
+      <c r="J11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1">
-        <v>2</v>
-      </c>
-      <c r="I12" s="6">
-        <v>2</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="6"/>
+        <v>176</v>
+      </c>
+      <c r="B12" s="48">
+        <v>27</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49">
+        <v>21</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49">
+        <v>19</v>
+      </c>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49">
+        <v>6</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="6"/>
+        <v>177</v>
+      </c>
+      <c r="B13" s="48">
+        <v>85</v>
+      </c>
+      <c r="C13" s="67"/>
+      <c r="D13" s="49">
+        <v>19</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49">
+        <v>16</v>
+      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49">
+        <v>9</v>
+      </c>
+      <c r="I13" s="50"/>
+      <c r="J13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="6">
-        <v>1</v>
-      </c>
+      <c r="I14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
       <c r="F15" s="1">
-        <v>6</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="6">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="44">
-        <v>7</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45">
-        <v>1</v>
-      </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45">
-        <v>8</v>
-      </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45">
-        <v>13</v>
-      </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="5">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>16</v>
-      </c>
-      <c r="G17" s="1">
-        <v>8</v>
-      </c>
-      <c r="H17" s="1">
-        <v>13</v>
-      </c>
-      <c r="I17" s="6">
-        <v>13</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>36</v>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5">
         <v>5</v>
       </c>
       <c r="C18" s="1">
-        <v>4</v>
-      </c>
-      <c r="D18" s="12">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>11</v>
-      </c>
-      <c r="G18" s="12">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
-        <v>13</v>
-      </c>
-      <c r="I18" s="6">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="1">
         <v>1</v>
       </c>
@@ -2408,343 +2404,341 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1">
-        <v>35</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="1">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="1">
-        <v>25</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="6">
-        <v>32</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="6">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="48">
+        <v>7</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49">
+        <v>1</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49">
+        <v>8</v>
+      </c>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49">
+        <v>13</v>
+      </c>
+      <c r="I19" s="50"/>
+      <c r="J19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G20" s="1">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="H20" s="1">
-        <v>14</v>
-      </c>
-      <c r="I20" s="22">
-        <v>14</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6">
-        <v>1</v>
-      </c>
-      <c r="L20" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
+        <v>13</v>
+      </c>
+      <c r="I20" s="6">
+        <v>13</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
       <c r="C21" s="1">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D21" s="12">
+        <v>2</v>
+      </c>
       <c r="E21" s="1">
-        <v>26</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1">
-        <v>36</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="22">
-        <v>14</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
+        <v>4</v>
+      </c>
+      <c r="F21" s="1">
+        <v>11</v>
+      </c>
+      <c r="G21" s="12">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>13</v>
+      </c>
+      <c r="I21" s="6">
+        <v>13</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="C22" s="1">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E22" s="1">
-        <v>14</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G22" s="1">
-        <v>14</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="6">
+        <v>32</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="5"/>
+        <v>145</v>
+      </c>
+      <c r="B23" s="5">
+        <v>43</v>
+      </c>
       <c r="C23" s="1">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="D23" s="1">
+        <v>17</v>
+      </c>
       <c r="E23" s="1">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="F23" s="1">
+        <v>11</v>
+      </c>
       <c r="G23" s="1">
-        <v>24</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
+        <v>27</v>
+      </c>
+      <c r="H23" s="1">
+        <v>14</v>
+      </c>
+      <c r="I23" s="22">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6">
+        <v>1</v>
+      </c>
+      <c r="L23" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A24" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <v>36</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="22">
+        <v>14</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="6"/>
       <c r="J25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="L25" s="46"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="44">
-        <v>1</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45">
-        <v>1</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45">
-        <v>1</v>
-      </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45">
-        <v>3</v>
-      </c>
-      <c r="I26" s="46"/>
-      <c r="J26" s="1">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6">
-        <v>1</v>
-      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>4</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>4</v>
-      </c>
-      <c r="H27" s="1">
-        <v>13</v>
-      </c>
-      <c r="I27" s="6">
-        <v>10</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>4</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12">
-        <v>4</v>
-      </c>
-      <c r="H28" s="1">
-        <v>12</v>
-      </c>
-      <c r="I28" s="6">
-        <v>10</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6">
-        <v>1</v>
+      <c r="B27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1">
-        <v>2</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1">
+        <v>24</v>
+      </c>
+      <c r="B29" s="48">
+        <v>1</v>
+      </c>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49">
+        <v>1</v>
+      </c>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49">
+        <v>1</v>
+      </c>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49">
         <v>3</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
-        <v>6</v>
-      </c>
-      <c r="H29" s="1">
-        <v>15</v>
-      </c>
-      <c r="I29" s="6">
-        <v>11</v>
-      </c>
+      <c r="I29" s="50"/>
       <c r="J29" s="1">
         <v>1</v>
       </c>
@@ -2754,153 +2748,147 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
       <c r="C30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>4</v>
+      </c>
+      <c r="H30" s="1">
+        <v>13</v>
+      </c>
+      <c r="I30" s="6">
+        <v>10</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1">
+        <v>12</v>
+      </c>
+      <c r="I31" s="6">
+        <v>10</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
         <v>3</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
         <v>6</v>
       </c>
-      <c r="H30" s="1">
-        <v>14</v>
-      </c>
-      <c r="I30" s="6">
-        <v>12</v>
-      </c>
-      <c r="J30" s="1">
-        <v>1</v>
-      </c>
-      <c r="K30" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>36</v>
+      <c r="H32" s="1">
+        <v>15</v>
+      </c>
+      <c r="I32" s="6">
+        <v>11</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B33" s="5"/>
       <c r="C33" s="1">
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="1">
-        <v>2</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1">
-        <v>2</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="H33" s="1">
+        <v>14</v>
+      </c>
+      <c r="I33" s="6">
+        <v>12</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+      <c r="K33" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="5">
-        <v>2</v>
+      <c r="B34" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="1">
-        <v>2</v>
+      <c r="D34" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="1">
-        <v>4</v>
+      <c r="F34" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>36</v>
@@ -2918,9 +2906,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>32</v>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>36</v>
@@ -2931,20 +2919,20 @@
       <c r="D35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="1">
-        <v>4</v>
+      <c r="E35" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="1">
-        <v>5</v>
+      <c r="G35" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I35" s="6">
-        <v>1</v>
+      <c r="I35" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>36</v>
@@ -2955,25 +2943,31 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="6">
-        <v>8</v>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>36</v>
@@ -2984,42 +2978,42 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
-      </c>
-      <c r="E37" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1">
-        <v>8</v>
-      </c>
-      <c r="H37" s="1">
-        <v>8</v>
-      </c>
-      <c r="I37" s="6">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K37" s="6">
-        <v>1</v>
+      <c r="K37" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>36</v>
@@ -3030,23 +3024,23 @@
       <c r="D38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
+      <c r="E38" s="1">
+        <v>4</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G38" s="1">
         <v>5</v>
       </c>
-      <c r="H38" s="1">
-        <v>8</v>
+      <c r="H38" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="I38" s="6">
-        <v>8</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>36</v>
@@ -3054,7 +3048,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>36</v>
@@ -3062,23 +3056,17 @@
       <c r="C39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="6">
         <v>8</v>
-      </c>
-      <c r="H39" s="1">
-        <v>6</v>
-      </c>
-      <c r="I39" s="6">
-        <v>14</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>36</v>
@@ -3089,57 +3077,179 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>8</v>
+      </c>
+      <c r="H40" s="1">
+        <v>8</v>
+      </c>
+      <c r="I40" s="6">
+        <v>22</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>5</v>
+      </c>
+      <c r="H41" s="1">
+        <v>8</v>
+      </c>
+      <c r="I41" s="6">
+        <v>8</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>8</v>
+      </c>
+      <c r="H42" s="1">
+        <v>6</v>
+      </c>
+      <c r="I42" s="6">
+        <v>14</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F40" s="10">
-        <v>1</v>
-      </c>
-      <c r="G40" s="10">
+      <c r="B43" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="10">
+        <v>1</v>
+      </c>
+      <c r="G43" s="10">
         <v>6</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H43" s="10">
         <v>6</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I43" s="11">
         <v>14</v>
       </c>
-      <c r="J40" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K40" s="11" t="s">
+      <c r="J43" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" s="11" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="L20:N23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="21">
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L23:N26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:K15 B16 D16 F16 H16 J16:K16 B17:K25 B26 D26 F26 H26 J26:K26 B27:K40">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"#"</formula>
+  <conditionalFormatting sqref="B11:E11 I22 C22 B23:C24 E23:E24 G22:G24 B12:B13 D12:D13">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="18"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF920000"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:K40">
+  <conditionalFormatting sqref="B3:K10 B14:K43 H11:H13 J11:K13 F11:F13">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3151,19 +3261,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:K25 B3:K15 B16 D16 F16 H16 J16:K16 B26 D26 F26 H26 J26:K26 B27:K40">
+  <conditionalFormatting sqref="B3:K10 F11:F13 H11:H13 J11:K13 B14:K18 B19 D19 F19 H19 J19:K19 B20:K28 B29 D29 F29 H29 J29:K29 B30:K43">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:K12 B29:K33 B36:K43 B14:K26 B13 D13 F13 H13 J13:K13">
     <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19 G19 I19 B20:C21 E20:E21 G20:G21">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="num" val="18"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF920000"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3230,22 +3335,22 @@
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="57"/>
+      <c r="B2" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="65"/>
       <c r="J2" s="31" t="s">
         <v>83</v>
       </c>
@@ -3264,19 +3369,19 @@
       <c r="B3" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="53"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="59"/>
       <c r="J3" s="27" t="s">
         <v>83</v>
       </c>
@@ -3356,18 +3461,18 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49" t="s">
+      <c r="D6" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="54"/>
       <c r="J6" s="33" t="s">
         <v>84</v>
       </c>
@@ -3689,18 +3794,18 @@
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="33" t="s">
         <v>79</v>
       </c>
@@ -3717,17 +3822,17 @@
         <v>58</v>
       </c>
       <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52" t="s">
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="53"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="27" t="s">
         <v>79</v>
       </c>
@@ -4000,54 +4105,54 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="58"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="50"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="54"/>
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="61"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="57"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49" t="s">
+      <c r="B31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="50"/>
+      <c r="I31" s="54"/>
       <c r="J31" s="33" t="s">
         <v>83</v>
       </c>
@@ -4066,19 +4171,19 @@
       <c r="B32" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52" t="s">
+      <c r="C32" s="58"/>
+      <c r="D32" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52" t="s">
+      <c r="E32" s="58"/>
+      <c r="F32" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52" t="s">
+      <c r="G32" s="58"/>
+      <c r="H32" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="I32" s="53"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="27" t="s">
         <v>83</v>
       </c>
@@ -4094,31 +4199,31 @@
       <c r="B33" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="D33" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="52" t="s">
+      <c r="D33" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="F33" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="52" t="s">
+      <c r="F33" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="H33" s="52" t="s">
+      <c r="H33" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="I33" s="53" t="s">
+      <c r="I33" s="59" t="s">
         <v>168</v>
       </c>
       <c r="J33" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="53" t="s">
+      <c r="K33" s="59" t="s">
         <v>78</v>
       </c>
       <c r="L33" s="18"/>
@@ -4131,15 +4236,15 @@
         <v>50</v>
       </c>
       <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="53"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
       <c r="J34" s="51"/>
-      <c r="K34" s="53"/>
+      <c r="K34" s="59"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
         <v>119</v>
@@ -4152,31 +4257,31 @@
       <c r="B35" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="52" t="s">
+      <c r="F35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="H35" s="52" t="s">
+      <c r="H35" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="I35" s="53" t="s">
+      <c r="I35" s="59" t="s">
         <v>168</v>
       </c>
       <c r="J35" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K35" s="53" t="s">
+      <c r="K35" s="59" t="s">
         <v>78</v>
       </c>
       <c r="L35" s="14"/>
@@ -4185,45 +4290,45 @@
       <c r="A36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="61"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="57"/>
       <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="58"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="50"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="54"/>
       <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="61"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="57"/>
       <c r="L38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -4261,7 +4366,7 @@
         <v>84</v>
       </c>
       <c r="L39" s="14"/>
-      <c r="M39" s="54" t="s">
+      <c r="M39" s="66" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4300,7 +4405,7 @@
         <v>84</v>
       </c>
       <c r="L40" s="14"/>
-      <c r="M40" s="54"/>
+      <c r="M40" s="66"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4337,7 +4442,7 @@
         <v>84</v>
       </c>
       <c r="L41" s="14"/>
-      <c r="M41" s="54"/>
+      <c r="M41" s="66"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4374,7 +4479,7 @@
         <v>84</v>
       </c>
       <c r="L42" s="14"/>
-      <c r="M42" s="54" t="s">
+      <c r="M42" s="66" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4413,7 +4518,7 @@
         <v>84</v>
       </c>
       <c r="L43" s="14"/>
-      <c r="M43" s="54"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -4450,7 +4555,7 @@
         <v>84</v>
       </c>
       <c r="L44" s="14"/>
-      <c r="M44" s="54"/>
+      <c r="M44" s="66"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -4588,47 +4693,47 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" s="51"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="53"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="59"/>
       <c r="J50" s="51"/>
-      <c r="K50" s="53"/>
+      <c r="K50" s="59"/>
       <c r="L50" s="14"/>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="59"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
-      <c r="H51" s="60"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="61"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="57"/>
       <c r="L51" s="14"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="50"/>
+      <c r="B52" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
       <c r="J52" s="33" t="s">
         <v>83</v>
       </c>
@@ -4647,13 +4752,13 @@
       <c r="B53" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="52"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="53"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="59"/>
       <c r="J53" s="27" t="s">
         <v>83</v>
       </c>
@@ -4672,13 +4777,13 @@
       <c r="B54" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="53"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="59"/>
       <c r="J54" s="27" t="s">
         <v>83</v>
       </c>
@@ -4697,13 +4802,13 @@
       <c r="B55" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="H55" s="52"/>
-      <c r="I55" s="53"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="59"/>
       <c r="J55" s="27" t="s">
         <v>83</v>
       </c>
@@ -4720,19 +4825,19 @@
         <v>159</v>
       </c>
       <c r="B56" s="51"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="I56" s="53"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" s="59"/>
       <c r="J56" s="27" t="s">
         <v>84</v>
       </c>
@@ -4749,19 +4854,19 @@
         <v>158</v>
       </c>
       <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52" t="s">
+      <c r="C57" s="58"/>
+      <c r="D57" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52" t="s">
+      <c r="E57" s="58"/>
+      <c r="F57" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="G57" s="52"/>
-      <c r="H57" s="52" t="s">
+      <c r="G57" s="58"/>
+      <c r="H57" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="I57" s="53"/>
+      <c r="I57" s="59"/>
       <c r="J57" s="27"/>
       <c r="K57" s="26"/>
       <c r="L57" s="14"/>
@@ -4777,19 +4882,19 @@
         <v>84</v>
       </c>
       <c r="C58" s="18"/>
-      <c r="D58" s="52" t="s">
+      <c r="D58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F58" s="52" t="s">
+      <c r="F58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="G58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H58" s="52" t="s">
+      <c r="H58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="I58" s="18" t="s">
@@ -4798,7 +4903,7 @@
       <c r="J58" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="K58" s="53" t="s">
+      <c r="K58" s="59" t="s">
         <v>84</v>
       </c>
       <c r="L58" s="14"/>
@@ -4812,20 +4917,20 @@
       </c>
       <c r="B59" s="51"/>
       <c r="C59" s="18"/>
-      <c r="D59" s="52"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="F59" s="52"/>
+      <c r="F59" s="58"/>
       <c r="G59" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="H59" s="52"/>
+      <c r="H59" s="58"/>
       <c r="I59" s="18" t="s">
         <v>154</v>
       </c>
       <c r="J59" s="51"/>
-      <c r="K59" s="53"/>
+      <c r="K59" s="59"/>
       <c r="L59" s="14"/>
       <c r="M59" s="19" t="s">
         <v>161</v>
@@ -4836,31 +4941,31 @@
         <v>156</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="52" t="s">
+      <c r="C60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="52" t="s">
+      <c r="E60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G60" s="52" t="s">
+      <c r="G60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="H60" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="I60" s="53" t="s">
+      <c r="I60" s="59" t="s">
         <v>84</v>
       </c>
       <c r="J60" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="K60" s="53" t="s">
+      <c r="K60" s="59" t="s">
         <v>84</v>
       </c>
       <c r="L60" s="13"/>
@@ -4873,69 +4978,69 @@
         <v>163</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="60"/>
+      <c r="C61" s="56"/>
       <c r="D61" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="E61" s="60"/>
+      <c r="E61" s="56"/>
       <c r="F61" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="G61" s="60"/>
+      <c r="G61" s="56"/>
       <c r="H61" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="I61" s="61"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="61"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="57"/>
       <c r="L61" s="14"/>
       <c r="M61" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="58"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="50"/>
-      <c r="J62" s="58"/>
-      <c r="K62" s="50"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="54"/>
       <c r="L62" s="14"/>
     </row>
     <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="59"/>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="60"/>
-      <c r="G63" s="60"/>
-      <c r="H63" s="60"/>
-      <c r="I63" s="61"/>
-      <c r="J63" s="59"/>
-      <c r="K63" s="61"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="57"/>
       <c r="L63" s="14"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49" t="s">
+      <c r="B64" s="52"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="50"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="53"/>
+      <c r="I64" s="54"/>
       <c r="J64" s="33" t="s">
         <v>81</v>
       </c>
@@ -4957,17 +5062,17 @@
       <c r="B65" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52"/>
-      <c r="F65" s="52" t="s">
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G65" s="52"/>
-      <c r="H65" s="52" t="s">
+      <c r="G65" s="58"/>
+      <c r="H65" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I65" s="53"/>
+      <c r="I65" s="59"/>
       <c r="J65" s="18" t="s">
         <v>81</v>
       </c>
@@ -4986,19 +5091,19 @@
       <c r="B66" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52" t="s">
+      <c r="C66" s="58"/>
+      <c r="D66" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="52"/>
-      <c r="H66" s="52" t="s">
+      <c r="G66" s="58"/>
+      <c r="H66" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I66" s="53"/>
+      <c r="I66" s="59"/>
       <c r="J66" s="27" t="s">
         <v>81</v>
       </c>
@@ -5017,19 +5122,19 @@
       <c r="B67" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E67" s="52"/>
-      <c r="F67" s="52" t="s">
+      <c r="C67" s="58"/>
+      <c r="D67" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="58"/>
+      <c r="F67" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G67" s="52"/>
-      <c r="H67" s="52" t="s">
+      <c r="G67" s="58"/>
+      <c r="H67" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I67" s="53"/>
+      <c r="I67" s="59"/>
       <c r="J67" s="27" t="s">
         <v>81</v>
       </c>
@@ -5069,19 +5174,19 @@
       <c r="B69" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="52"/>
-      <c r="D69" s="52" t="s">
+      <c r="C69" s="58"/>
+      <c r="D69" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="E69" s="52"/>
-      <c r="F69" s="52" t="s">
+      <c r="E69" s="58"/>
+      <c r="F69" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="G69" s="52"/>
-      <c r="H69" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="I69" s="53"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I69" s="59"/>
       <c r="J69" s="27" t="s">
         <v>83</v>
       </c>
@@ -5097,20 +5202,20 @@
       <c r="A70" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B70" s="58"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="G70" s="49"/>
-      <c r="H70" s="49"/>
-      <c r="I70" s="49"/>
-      <c r="J70" s="49"/>
-      <c r="K70" s="50"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="54"/>
       <c r="L70" s="14"/>
-      <c r="M70" s="54" t="s">
+      <c r="M70" s="66" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5121,15 +5226,15 @@
       <c r="B71" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="52"/>
-      <c r="D71" s="52" t="s">
+      <c r="C71" s="58"/>
+      <c r="D71" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="E71" s="52"/>
-      <c r="F71" s="52"/>
-      <c r="G71" s="52"/>
-      <c r="H71" s="52"/>
-      <c r="I71" s="53"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="59"/>
       <c r="J71" s="27" t="s">
         <v>141</v>
       </c>
@@ -5137,22 +5242,22 @@
         <v>141</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="54"/>
+      <c r="M71" s="66"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B72" s="51"/>
-      <c r="C72" s="52"/>
-      <c r="D72" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="G72" s="52"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="53"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="59"/>
       <c r="J72" s="27"/>
       <c r="K72" s="26"/>
       <c r="L72" s="14"/>
@@ -5165,15 +5270,15 @@
         <v>143</v>
       </c>
       <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="53"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="58"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="59"/>
       <c r="J73" s="27"/>
       <c r="K73" s="26"/>
       <c r="L73" s="14"/>
@@ -5185,18 +5290,18 @@
       <c r="A74" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="59"/>
-      <c r="C74" s="60"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="60" t="s">
+      <c r="B74" s="55"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G74" s="60"/>
-      <c r="H74" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="I74" s="61"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="I74" s="57"/>
       <c r="J74" s="29" t="s">
         <v>83</v>
       </c>
@@ -5215,19 +5320,19 @@
       <c r="B75" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="52"/>
-      <c r="D75" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E75" s="52"/>
-      <c r="F75" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G75" s="52"/>
-      <c r="H75" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="I75" s="53"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I75" s="59"/>
       <c r="J75" s="27" t="s">
         <v>83</v>
       </c>
@@ -5243,22 +5348,22 @@
       <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" s="63"/>
-      <c r="F76" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="I76" s="64"/>
+      <c r="B76" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="I76" s="62"/>
       <c r="J76" s="40" t="s">
         <v>83</v>
       </c>
@@ -5272,6 +5377,109 @@
     </row>
   </sheetData>
   <mergeCells count="127">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="M39:M41"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="M70:M71"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="J62:K63"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D64:I64"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B62:I63"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:K70"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="B29:I30"/>
     <mergeCell ref="J29:K30"/>
@@ -5296,109 +5504,6 @@
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:K70"/>
-    <mergeCell ref="J62:K63"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D64:I64"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B62:I63"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="K58:K59"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="M70:M71"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5545,7 +5650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42270057-09F5-4DBC-B29A-71117FFFAFC1}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -5555,11 +5660,11 @@
     <col min="2" max="2" width="29.5703125" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="45" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor fixes + better U64ToF32
The major change is to the unsigned 64-bit integer to single precision float conversion. It use to be the slowest.
- Added new methods to the performance benchmark: fused-add-add, with float80, and 2Sum based methods
- Improved U64 => f32 performance (~5%-30%)
- Updated the benchmark excel files and instruction matrix to reflect these changes

The minor changes:
- Various minor typo/better comment explanations
- Added "shuffle viaXor" visualization
- Added divByScalar benchmark (I forgot to add eariler)
- New minor methods to benchmarks
</commit_message>
<xml_diff>
--- a/external/InstructionCost.xlsx
+++ b/external/InstructionCost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AECE3A-69BF-4448-B117-DD52DF272024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706FFFB-78DB-4B8D-A61D-2338C3CC4661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
   </bookViews>
@@ -371,7 +371,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="178">
   <si>
     <t>s8</t>
   </si>
@@ -697,9 +697,6 @@
     <t>hsubs</t>
   </si>
   <si>
-    <t>maddubs/madd</t>
-  </si>
-  <si>
     <t>sad</t>
   </si>
   <si>
@@ -905,6 +902,9 @@
   </si>
   <si>
     <t>shuffle by vector</t>
+  </si>
+  <si>
+    <t>madd[ubs]</t>
   </si>
 </sst>
 </file>
@@ -1352,48 +1352,60 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1402,18 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1863,8 +1863,8 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:C12"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2185,24 +2185,24 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="48">
         <v>25</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46">
         <v>17</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49">
+      <c r="E11" s="46"/>
+      <c r="F11" s="46">
         <v>12</v>
       </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49">
+      <c r="G11" s="46"/>
+      <c r="H11" s="46">
         <v>6</v>
       </c>
-      <c r="I11" s="50"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2212,24 +2212,24 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="48">
         <v>27</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49">
+      <c r="C12" s="46"/>
+      <c r="D12" s="46">
         <v>21</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49">
+      <c r="E12" s="46"/>
+      <c r="F12" s="46">
         <v>19</v>
       </c>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49">
+      <c r="G12" s="46"/>
+      <c r="H12" s="46">
         <v>6</v>
       </c>
-      <c r="I12" s="50"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2239,24 +2239,24 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="48">
         <v>85</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46">
         <v>19</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49">
+      <c r="E13" s="46"/>
+      <c r="F13" s="46">
         <v>16</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49">
+      <c r="G13" s="46"/>
+      <c r="H13" s="46">
         <v>9</v>
       </c>
-      <c r="I13" s="50"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2406,19 +2406,19 @@
       <c r="B19" s="48">
         <v>7</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49">
-        <v>1</v>
-      </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49">
+      <c r="C19" s="46"/>
+      <c r="D19" s="46">
+        <v>1</v>
+      </c>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46">
         <v>8</v>
       </c>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49">
+      <c r="G19" s="46"/>
+      <c r="H19" s="46">
         <v>13</v>
       </c>
-      <c r="I19" s="50"/>
+      <c r="I19" s="47"/>
       <c r="J19" s="1" t="s">
         <v>36</v>
       </c>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="5">
         <v>43</v>
@@ -2565,15 +2565,15 @@
       <c r="K23" s="6">
         <v>1</v>
       </c>
-      <c r="L23" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
+      <c r="L23" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="1">
@@ -2593,13 +2593,13 @@
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="1">
@@ -2621,13 +2621,13 @@
       <c r="K25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="46"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="1">
@@ -2645,9 +2645,9 @@
       <c r="I26" s="6"/>
       <c r="J26" s="1"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
@@ -2723,19 +2723,19 @@
       <c r="B29" s="48">
         <v>1</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49">
-        <v>1</v>
-      </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49">
-        <v>1</v>
-      </c>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49">
+      <c r="C29" s="46"/>
+      <c r="D29" s="46">
+        <v>1</v>
+      </c>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46">
+        <v>1</v>
+      </c>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46">
         <v>3</v>
       </c>
-      <c r="I29" s="50"/>
+      <c r="I29" s="47"/>
       <c r="J29" s="1">
         <v>1</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>8</v>
       </c>
       <c r="I40" s="6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>36</v>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>36</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>36</v>
@@ -3214,6 +3214,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L23:N26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
@@ -3230,11 +3235,6 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L23:N26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:E11 I22 C22 B23:C24 E23:E24 G22:G24 B12:B13 D12:D13">
     <cfRule type="colorScale" priority="10">
@@ -3279,8 +3279,8 @@
   <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N72" sqref="N72"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,22 +3332,22 @@
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="65"/>
+      <c r="B2" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="62"/>
       <c r="J2" s="31" t="s">
         <v>83</v>
       </c>
@@ -3366,19 +3366,19 @@
       <c r="B3" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="59"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="52"/>
       <c r="J3" s="27" t="s">
         <v>83</v>
       </c>
@@ -3458,18 +3458,18 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53" t="s">
+      <c r="D6" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="54"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" s="56"/>
       <c r="J6" s="33" t="s">
         <v>84</v>
       </c>
@@ -3555,7 +3555,7 @@
       <c r="K9" s="39"/>
       <c r="L9" s="14"/>
       <c r="M9" s="19" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
         <v>84</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>84</v>
@@ -3667,8 +3667,12 @@
       <c r="I13" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="26"/>
+      <c r="J13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>81</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="19" t="s">
         <v>103</v>
@@ -3702,8 +3706,12 @@
       <c r="I14" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="26"/>
+      <c r="J14" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>81</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="19" t="s">
         <v>47</v>
@@ -3732,10 +3740,10 @@
         <v>81</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>83</v>
@@ -3771,10 +3779,10 @@
         <v>81</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>83</v>
@@ -3791,18 +3799,18 @@
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53" t="s">
+      <c r="B17" s="63"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53" t="s">
+      <c r="E17" s="55"/>
+      <c r="F17" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="33" t="s">
         <v>79</v>
       </c>
@@ -3819,17 +3827,17 @@
         <v>58</v>
       </c>
       <c r="B18" s="51"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58" t="s">
+      <c r="E18" s="57"/>
+      <c r="F18" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="27" t="s">
         <v>79</v>
       </c>
@@ -3855,8 +3863,12 @@
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>84</v>
+      </c>
       <c r="L19" s="14"/>
       <c r="M19" s="19" t="s">
         <v>106</v>
@@ -3876,8 +3888,12 @@
       <c r="G20" s="30"/>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="28"/>
+      <c r="J20" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="L20" s="14"/>
       <c r="M20" s="19" t="s">
         <v>107</v>
@@ -3901,7 +3917,7 @@
       <c r="K21" s="26"/>
       <c r="L21" s="14"/>
       <c r="M21" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -3922,7 +3938,7 @@
       <c r="K22" s="26"/>
       <c r="L22" s="14"/>
       <c r="M22" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -3943,7 +3959,7 @@
       <c r="K23" s="26"/>
       <c r="L23" s="14"/>
       <c r="M23" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3976,7 +3992,7 @@
       <c r="K24" s="26"/>
       <c r="L24" s="14"/>
       <c r="M24" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -4013,7 +4029,7 @@
       <c r="K25" s="35"/>
       <c r="L25" s="14"/>
       <c r="M25" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -4048,11 +4064,11 @@
         <v>83</v>
       </c>
       <c r="K26" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -4075,7 +4091,7 @@
       </c>
       <c r="L27" s="14"/>
       <c r="M27" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -4098,58 +4114,58 @@
       </c>
       <c r="L28" s="14"/>
       <c r="M28" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="52"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="54"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="56"/>
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="57"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="54"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53" t="s">
+      <c r="B31" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="54"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="33" t="s">
         <v>83</v>
       </c>
@@ -4158,7 +4174,7 @@
       </c>
       <c r="L31" s="14"/>
       <c r="M31" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -4166,21 +4182,21 @@
         <v>53</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="I32" s="59"/>
+        <v>167</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="I32" s="52"/>
       <c r="J32" s="27" t="s">
         <v>83</v>
       </c>
@@ -4196,36 +4212,36 @@
       <c r="B33" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="F33" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="H33" s="58" t="s">
+      <c r="C33" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="H33" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="I33" s="59" t="s">
-        <v>168</v>
+      <c r="I33" s="52" t="s">
+        <v>167</v>
       </c>
       <c r="J33" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="59" t="s">
+      <c r="K33" s="52" t="s">
         <v>78</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -4233,18 +4249,18 @@
         <v>50</v>
       </c>
       <c r="B34" s="51"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="59"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="52"/>
       <c r="J34" s="51"/>
-      <c r="K34" s="59"/>
+      <c r="K34" s="52"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -4252,33 +4268,33 @@
         <v>51</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="C35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="G35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="H35" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="I35" s="59" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="I35" s="52" t="s">
+        <v>167</v>
       </c>
       <c r="J35" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K35" s="59" t="s">
+      <c r="K35" s="52" t="s">
         <v>78</v>
       </c>
       <c r="L35" s="14"/>
@@ -4287,45 +4303,45 @@
       <c r="A36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="57"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="54"/>
       <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="54"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="56"/>
       <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="57"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="54"/>
       <c r="L38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -4363,8 +4379,8 @@
         <v>84</v>
       </c>
       <c r="L39" s="14"/>
-      <c r="M39" s="66" t="s">
-        <v>120</v>
+      <c r="M39" s="58" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -4402,7 +4418,7 @@
         <v>84</v>
       </c>
       <c r="L40" s="14"/>
-      <c r="M40" s="66"/>
+      <c r="M40" s="58"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4439,7 +4455,7 @@
         <v>84</v>
       </c>
       <c r="L41" s="14"/>
-      <c r="M41" s="66"/>
+      <c r="M41" s="58"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4476,8 +4492,8 @@
         <v>84</v>
       </c>
       <c r="L42" s="14"/>
-      <c r="M42" s="66" t="s">
-        <v>121</v>
+      <c r="M42" s="58" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -4515,7 +4531,7 @@
         <v>84</v>
       </c>
       <c r="L43" s="14"/>
-      <c r="M43" s="66"/>
+      <c r="M43" s="58"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -4552,7 +4568,7 @@
         <v>84</v>
       </c>
       <c r="L44" s="14"/>
-      <c r="M44" s="66"/>
+      <c r="M44" s="58"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -4582,7 +4598,7 @@
       </c>
       <c r="L45" s="14"/>
       <c r="M45" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -4597,13 +4613,13 @@
         <v>78</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J46" s="27" t="s">
         <v>84</v>
@@ -4613,7 +4629,7 @@
       </c>
       <c r="L46" s="14"/>
       <c r="M46" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -4628,13 +4644,13 @@
         <v>78</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J47" s="27" t="s">
         <v>78</v>
@@ -4644,7 +4660,7 @@
       </c>
       <c r="L47" s="14"/>
       <c r="M47" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -4669,12 +4685,12 @@
       </c>
       <c r="L48" s="14"/>
       <c r="M48" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B49" s="27"/>
       <c r="C49" s="18"/>
@@ -4690,47 +4706,47 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" s="51"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="59"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="52"/>
       <c r="J50" s="51"/>
-      <c r="K50" s="59"/>
+      <c r="K50" s="52"/>
       <c r="L50" s="14"/>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="57"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="54"/>
       <c r="L51" s="14"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="54"/>
+      <c r="B52" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="56"/>
       <c r="J52" s="33" t="s">
         <v>83</v>
       </c>
@@ -4749,13 +4765,13 @@
       <c r="B53" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="59"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="52"/>
       <c r="J53" s="27" t="s">
         <v>83</v>
       </c>
@@ -4774,13 +4790,13 @@
       <c r="B54" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="52"/>
       <c r="J54" s="27" t="s">
         <v>83</v>
       </c>
@@ -4799,13 +4815,13 @@
       <c r="B55" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="59"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="52"/>
       <c r="J55" s="27" t="s">
         <v>83</v>
       </c>
@@ -4819,225 +4835,215 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" s="51"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="I56" s="59"/>
-      <c r="J56" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="K56" s="26" t="s">
-        <v>84</v>
-      </c>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="57"/>
+      <c r="F56" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" s="52"/>
+      <c r="J56" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="K56" s="52"/>
       <c r="L56" s="14"/>
       <c r="M56" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B57" s="51"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="I57" s="59"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="26"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="I57" s="52"/>
+      <c r="J57" s="51"/>
+      <c r="K57" s="52"/>
       <c r="L57" s="14"/>
       <c r="M57" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B58" s="51" t="s">
         <v>84</v>
       </c>
       <c r="C58" s="18"/>
-      <c r="D58" s="58" t="s">
+      <c r="D58" s="57" t="s">
         <v>84</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F58" s="58" t="s">
+      <c r="F58" s="57" t="s">
         <v>84</v>
       </c>
       <c r="G58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H58" s="58" t="s">
+      <c r="H58" s="57" t="s">
         <v>84</v>
       </c>
       <c r="I58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J58" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="K58" s="59" t="s">
-        <v>84</v>
-      </c>
+      <c r="J58" s="51"/>
+      <c r="K58" s="52"/>
       <c r="L58" s="14"/>
       <c r="M58" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B59" s="51"/>
       <c r="C59" s="18"/>
-      <c r="D59" s="58"/>
+      <c r="D59" s="57"/>
       <c r="E59" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="F59" s="58"/>
+        <v>167</v>
+      </c>
+      <c r="F59" s="57"/>
       <c r="G59" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="H59" s="58"/>
+        <v>153</v>
+      </c>
+      <c r="H59" s="57"/>
       <c r="I59" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J59" s="51"/>
-      <c r="K59" s="59"/>
+      <c r="K59" s="52"/>
       <c r="L59" s="14"/>
       <c r="M59" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="58" t="s">
+      <c r="C60" s="57" t="s">
         <v>84</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="58" t="s">
+      <c r="E60" s="57" t="s">
         <v>84</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G60" s="58" t="s">
+      <c r="G60" s="57" t="s">
         <v>84</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="I60" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="J60" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="K60" s="59" t="s">
-        <v>84</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="I60" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="J60" s="51"/>
+      <c r="K60" s="52"/>
       <c r="L60" s="13"/>
       <c r="M60" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="56"/>
+      <c r="C61" s="59"/>
       <c r="D61" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E61" s="56"/>
+        <v>167</v>
+      </c>
+      <c r="E61" s="59"/>
       <c r="F61" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="G61" s="56"/>
+        <v>153</v>
+      </c>
+      <c r="G61" s="59"/>
       <c r="H61" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="I61" s="57"/>
-      <c r="J61" s="55"/>
-      <c r="K61" s="57"/>
+        <v>167</v>
+      </c>
+      <c r="I61" s="54"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="54"/>
       <c r="L61" s="14"/>
       <c r="M61" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="52"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="53"/>
-      <c r="H62" s="53"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="54"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="56"/>
+      <c r="J62" s="63"/>
+      <c r="K62" s="56"/>
       <c r="L62" s="14"/>
     </row>
     <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="57"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="57"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="59"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="59"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="54"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="54"/>
       <c r="L63" s="14"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="52"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53" t="s">
+      <c r="B64" s="63"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="53"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="53"/>
-      <c r="I64" s="54"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="56"/>
       <c r="J64" s="33" t="s">
         <v>81</v>
       </c>
@@ -5046,10 +5052,10 @@
       </c>
       <c r="L64" s="14"/>
       <c r="M64" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N64" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -5059,17 +5065,17 @@
       <c r="B65" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58" t="s">
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58" t="s">
+      <c r="G65" s="57"/>
+      <c r="H65" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="I65" s="59"/>
+      <c r="I65" s="52"/>
       <c r="J65" s="18" t="s">
         <v>81</v>
       </c>
@@ -5078,7 +5084,7 @@
       </c>
       <c r="L65" s="14"/>
       <c r="M65" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -5088,19 +5094,19 @@
       <c r="B66" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="58"/>
-      <c r="F66" s="58" t="s">
+      <c r="C66" s="57"/>
+      <c r="D66" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="58"/>
-      <c r="H66" s="58" t="s">
+      <c r="G66" s="57"/>
+      <c r="H66" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="I66" s="59"/>
+      <c r="I66" s="52"/>
       <c r="J66" s="27" t="s">
         <v>81</v>
       </c>
@@ -5109,29 +5115,29 @@
       </c>
       <c r="L66" s="14"/>
       <c r="M66" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B67" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58" t="s">
+      <c r="C67" s="57"/>
+      <c r="D67" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="57"/>
+      <c r="F67" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58" t="s">
+      <c r="G67" s="57"/>
+      <c r="H67" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="I67" s="59"/>
+      <c r="I67" s="52"/>
       <c r="J67" s="27" t="s">
         <v>81</v>
       </c>
@@ -5140,7 +5146,7 @@
       </c>
       <c r="L67" s="14"/>
       <c r="M67" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -5161,7 +5167,7 @@
       <c r="K68" s="26"/>
       <c r="L68" s="14"/>
       <c r="M68" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -5171,19 +5177,19 @@
       <c r="B69" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58" t="s">
+      <c r="C69" s="57"/>
+      <c r="D69" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="E69" s="57"/>
+      <c r="F69" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="I69" s="59"/>
+      <c r="G69" s="57"/>
+      <c r="H69" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I69" s="52"/>
       <c r="J69" s="27" t="s">
         <v>83</v>
       </c>
@@ -5192,113 +5198,113 @@
       </c>
       <c r="L69" s="14"/>
       <c r="M69" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B70" s="52"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="54"/>
+        <v>138</v>
+      </c>
+      <c r="B70" s="63"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="G70" s="55"/>
+      <c r="H70" s="55"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="56"/>
       <c r="L70" s="14"/>
-      <c r="M70" s="66" t="s">
-        <v>134</v>
+      <c r="M70" s="58" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B71" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="E71" s="58"/>
-      <c r="F71" s="58"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="59"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="E71" s="57"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="57"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="52"/>
       <c r="J71" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K71" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="66"/>
+      <c r="M71" s="58"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B72" s="51"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="59"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="57"/>
+      <c r="F72" s="57"/>
+      <c r="G72" s="57"/>
+      <c r="H72" s="57"/>
+      <c r="I72" s="52"/>
       <c r="J72" s="27"/>
       <c r="K72" s="26"/>
       <c r="L72" s="14"/>
       <c r="M72" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B73" s="51"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E73" s="58"/>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="59"/>
+      <c r="C73" s="57"/>
+      <c r="D73" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="57"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="57"/>
+      <c r="H73" s="57"/>
+      <c r="I73" s="52"/>
       <c r="J73" s="27"/>
       <c r="K73" s="26"/>
       <c r="L73" s="14"/>
       <c r="M73" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56" t="s">
+      <c r="B74" s="53"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="I74" s="57"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="I74" s="54"/>
       <c r="J74" s="29" t="s">
         <v>83</v>
       </c>
@@ -5307,7 +5313,7 @@
       </c>
       <c r="L74" s="14"/>
       <c r="M74" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -5317,19 +5323,19 @@
       <c r="B75" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="I75" s="59"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="57"/>
+      <c r="F75" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="57"/>
+      <c r="H75" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I75" s="52"/>
       <c r="J75" s="27" t="s">
         <v>83</v>
       </c>
@@ -5338,29 +5344,29 @@
       </c>
       <c r="L75" s="14"/>
       <c r="M75" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" s="61"/>
-      <c r="F76" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="G76" s="61"/>
-      <c r="H76" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="I76" s="62"/>
+      <c r="B76" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="65"/>
+      <c r="D76" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="65"/>
+      <c r="F76" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="I76" s="66"/>
       <c r="J76" s="40" t="s">
         <v>83</v>
       </c>
@@ -5369,35 +5375,63 @@
       </c>
       <c r="L76" s="14"/>
       <c r="M76" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="127">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="M70:M71"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
+  <mergeCells count="124">
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B29:I30"/>
+    <mergeCell ref="J29:K30"/>
+    <mergeCell ref="B37:I38"/>
+    <mergeCell ref="J37:K38"/>
+    <mergeCell ref="B50:I51"/>
+    <mergeCell ref="J50:K51"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:K70"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -5422,6 +5456,16 @@
     <mergeCell ref="B53:I53"/>
     <mergeCell ref="I33:I34"/>
     <mergeCell ref="B35:B36"/>
+    <mergeCell ref="M39:M41"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="M70:M71"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="J62:K63"/>
     <mergeCell ref="B54:I54"/>
     <mergeCell ref="B55:I55"/>
@@ -5436,71 +5480,30 @@
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="F58:F59"/>
     <mergeCell ref="H58:H59"/>
+    <mergeCell ref="J56:K61"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="G60:G61"/>
     <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="K58:K59"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="D67:E67"/>
     <mergeCell ref="F67:G67"/>
     <mergeCell ref="H67:I67"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:K70"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B29:I30"/>
-    <mergeCell ref="J29:K30"/>
-    <mergeCell ref="B37:I38"/>
-    <mergeCell ref="J37:K38"/>
-    <mergeCell ref="B50:I51"/>
-    <mergeCell ref="J50:K51"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5619,7 +5622,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B2:B3 D2:D3 F2:F3 H2:H3 J2:L3 B4:L5 B6:D6 F6 H6 J6:L6 B7:L16 M8:M9 B17:B18 D17:D18 F17:F18 H17:H18 J17:L18 B19:L28 B29 J29 B31:B32 D31:D32 F31:F32 H31:H32 J31:L32 B33:L33 B35:L35 B37 J37 B39:L49 B50 J50 B52:B58 J52:L58 D56:D57 F56:F58 H56:H58 B58:L58 C59 E59 G59 I59 L59 B60:L60 B60:B62 D61 F61 H61 L61 J62 N64 B64:B67 D64:D67 J64:L67 F65:F67 H65:H67 B68:L68 H69 J69:L69 B69:B76 D69:D76 F69:F76 H71:H76 J71:L76</xm:sqref>
+          <xm:sqref>B2:B3 D2:D3 F2:F3 H2:H3 J2:L3 B4:L5 B6:D6 F6 H6 J6:L6 B7:L16 M8:M9 B17:B18 D17:D18 F17:F18 H17:H18 J17:L18 B19:L28 B29 J29 B31:B32 D31:D32 F31:F32 H31:H32 J31:L32 B33:L33 B35:L35 B37 J37 B39:L49 B50 J50 J52:L55 B52:B58 J56 D56:D57 F56:F58 H56:H58 L56:L61 B58:I58 C59 E59 G59 I59 B60:I60 B60:B62 D61 F61 H61 J62 N64 B64:B67 D64:D67 J64:L67 F65:F67 H65:H67 B68:L68 H69 J69:L69 B69:B76 D69:D76 F69:F76 H71:H76 J71:L76</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5635,7 +5638,7 @@
           <x14:formula1>
             <xm:f>enums!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F76 I7:I31 C2:C31 G72:G76 D2:D76 E2:E31 H2:H76 E72:E76 G2:G31 C72:C76 J2:K76 B60:B76 B2:B58 I2:I5 C33:C70 E33:E70 G33:G70 I33:I70 I72:I76</xm:sqref>
+          <xm:sqref>F2:F76 I7:I31 C2:C31 G72:G76 D2:D76 E2:E31 H2:H76 E72:E76 G2:G31 C72:C76 I72:I76 B60:B76 B2:B58 I2:I5 C33:C70 E33:E70 G33:G70 I33:I70 K62:K76 K2:K55 J2:J56 J62:J76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5659,10 +5662,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>173</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5702,43 +5705,43 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor cmpGrt improve + instruction image
- Modified the unsigned 64-bit compare methods to use bit manipulation rather then a call to `_either`. clang already does this.
- Updated the minimal instruction cost to reflect current optimizations
- Fixed the full image to include the column name
</commit_message>
<xml_diff>
--- a/external/InstructionCost.xlsx
+++ b/external/InstructionCost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706FFFB-78DB-4B8D-A61D-2338C3CC4661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABE5FC8-EB51-4731-BEC9-D58435FF7990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0228E47D-794C-431C-A2A8-62B0A8D25E03}"/>
   </bookViews>
   <sheets>
     <sheet name="Emulated" sheetId="1" r:id="rId1"/>
@@ -1352,68 +1352,68 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1864,7 +1864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,19 +2190,19 @@
       <c r="B11" s="48">
         <v>25</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46">
+      <c r="C11" s="49"/>
+      <c r="D11" s="49">
         <v>17</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46">
+      <c r="E11" s="49"/>
+      <c r="F11" s="49">
         <v>12</v>
       </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46">
+      <c r="G11" s="49"/>
+      <c r="H11" s="49">
         <v>6</v>
       </c>
-      <c r="I11" s="47"/>
+      <c r="I11" s="50"/>
       <c r="J11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2217,19 +2217,19 @@
       <c r="B12" s="48">
         <v>27</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49">
         <v>21</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46">
+      <c r="E12" s="49"/>
+      <c r="F12" s="49">
         <v>19</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46">
+      <c r="G12" s="49"/>
+      <c r="H12" s="49">
         <v>6</v>
       </c>
-      <c r="I12" s="47"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2244,19 +2244,19 @@
       <c r="B13" s="48">
         <v>85</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49">
         <v>19</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46">
+      <c r="E13" s="49"/>
+      <c r="F13" s="49">
         <v>16</v>
       </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46">
+      <c r="G13" s="49"/>
+      <c r="H13" s="49">
         <v>9</v>
       </c>
-      <c r="I13" s="47"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2406,19 +2406,19 @@
       <c r="B19" s="48">
         <v>7</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46">
-        <v>1</v>
-      </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46">
+      <c r="C19" s="49"/>
+      <c r="D19" s="49">
+        <v>1</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49">
         <v>8</v>
       </c>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46">
+      <c r="G19" s="49"/>
+      <c r="H19" s="49">
         <v>13</v>
       </c>
-      <c r="I19" s="47"/>
+      <c r="I19" s="50"/>
       <c r="J19" s="1" t="s">
         <v>36</v>
       </c>
@@ -2565,11 +2565,11 @@
       <c r="K23" s="6">
         <v>1</v>
       </c>
-      <c r="L23" s="49" t="s">
+      <c r="L23" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -2593,9 +2593,9 @@
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -2621,9 +2621,9 @@
       <c r="K25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -2645,9 +2645,9 @@
       <c r="I26" s="6"/>
       <c r="J26" s="1"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
@@ -2723,19 +2723,19 @@
       <c r="B29" s="48">
         <v>1</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46">
-        <v>1</v>
-      </c>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46">
-        <v>1</v>
-      </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46">
+      <c r="C29" s="49"/>
+      <c r="D29" s="49">
+        <v>1</v>
+      </c>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49">
+        <v>1</v>
+      </c>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49">
         <v>3</v>
       </c>
-      <c r="I29" s="47"/>
+      <c r="I29" s="50"/>
       <c r="J29" s="1">
         <v>1</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>4</v>
       </c>
       <c r="H30" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I30" s="6">
         <v>10</v>
@@ -2801,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I31" s="6">
         <v>10</v>
@@ -2830,7 +2830,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I32" s="6">
         <v>11</v>
@@ -2859,7 +2859,7 @@
         <v>6</v>
       </c>
       <c r="H33" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I33" s="6">
         <v>12</v>
@@ -3214,11 +3214,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="L23:N26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
@@ -3235,6 +3230,11 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L23:N26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:E11 I22 C22 B23:C24 E23:E24 G22:G24 B12:B13 D12:D13">
     <cfRule type="colorScale" priority="10">
@@ -3332,22 +3332,22 @@
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="62"/>
+      <c r="B2" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="65"/>
       <c r="J2" s="31" t="s">
         <v>83</v>
       </c>
@@ -3366,19 +3366,19 @@
       <c r="B3" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="52"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="59"/>
       <c r="J3" s="27" t="s">
         <v>83</v>
       </c>
@@ -3458,18 +3458,18 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55" t="s">
+      <c r="D6" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="I6" s="56"/>
+      <c r="I6" s="54"/>
       <c r="J6" s="33" t="s">
         <v>84</v>
       </c>
@@ -3799,18 +3799,18 @@
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="33" t="s">
         <v>79</v>
       </c>
@@ -3827,17 +3827,17 @@
         <v>58</v>
       </c>
       <c r="B18" s="51"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57" t="s">
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="52"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="27" t="s">
         <v>79</v>
       </c>
@@ -4118,54 +4118,54 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="63"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="56"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="54"/>
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="54"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="57"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55" t="s">
+      <c r="B31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="56"/>
+      <c r="I31" s="54"/>
       <c r="J31" s="33" t="s">
         <v>83</v>
       </c>
@@ -4184,19 +4184,19 @@
       <c r="B32" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57" t="s">
+      <c r="C32" s="58"/>
+      <c r="D32" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57" t="s">
+      <c r="E32" s="58"/>
+      <c r="F32" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57" t="s">
+      <c r="G32" s="58"/>
+      <c r="H32" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="I32" s="52"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="27" t="s">
         <v>83</v>
       </c>
@@ -4212,31 +4212,31 @@
       <c r="B33" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="D33" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="57" t="s">
+      <c r="D33" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="F33" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="57" t="s">
+      <c r="F33" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="H33" s="57" t="s">
+      <c r="H33" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="I33" s="52" t="s">
+      <c r="I33" s="59" t="s">
         <v>167</v>
       </c>
       <c r="J33" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="59" t="s">
         <v>78</v>
       </c>
       <c r="L33" s="18"/>
@@ -4249,15 +4249,15 @@
         <v>50</v>
       </c>
       <c r="B34" s="51"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="52"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
       <c r="J34" s="51"/>
-      <c r="K34" s="52"/>
+      <c r="K34" s="59"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
         <v>118</v>
@@ -4270,31 +4270,31 @@
       <c r="B35" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="57" t="s">
+      <c r="D35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="57" t="s">
+      <c r="E35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="F35" s="57" t="s">
+      <c r="F35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="G35" s="57" t="s">
+      <c r="G35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="H35" s="57" t="s">
+      <c r="H35" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="I35" s="52" t="s">
+      <c r="I35" s="59" t="s">
         <v>167</v>
       </c>
       <c r="J35" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K35" s="52" t="s">
+      <c r="K35" s="59" t="s">
         <v>78</v>
       </c>
       <c r="L35" s="14"/>
@@ -4303,45 +4303,45 @@
       <c r="A36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="54"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="57"/>
       <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="63"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="56"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="54"/>
       <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="54"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="57"/>
       <c r="L38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -4379,7 +4379,7 @@
         <v>84</v>
       </c>
       <c r="L39" s="14"/>
-      <c r="M39" s="58" t="s">
+      <c r="M39" s="66" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4418,7 +4418,7 @@
         <v>84</v>
       </c>
       <c r="L40" s="14"/>
-      <c r="M40" s="58"/>
+      <c r="M40" s="66"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4455,7 +4455,7 @@
         <v>84</v>
       </c>
       <c r="L41" s="14"/>
-      <c r="M41" s="58"/>
+      <c r="M41" s="66"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4492,7 +4492,7 @@
         <v>84</v>
       </c>
       <c r="L42" s="14"/>
-      <c r="M42" s="58" t="s">
+      <c r="M42" s="66" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4531,7 +4531,7 @@
         <v>84</v>
       </c>
       <c r="L43" s="14"/>
-      <c r="M43" s="58"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -4568,7 +4568,7 @@
         <v>84</v>
       </c>
       <c r="L44" s="14"/>
-      <c r="M44" s="58"/>
+      <c r="M44" s="66"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -4706,47 +4706,47 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B50" s="51"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="52"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="59"/>
       <c r="J50" s="51"/>
-      <c r="K50" s="52"/>
+      <c r="K50" s="59"/>
       <c r="L50" s="14"/>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="53"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="54"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="57"/>
       <c r="L51" s="14"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="56"/>
+      <c r="B52" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
       <c r="J52" s="33" t="s">
         <v>83</v>
       </c>
@@ -4765,13 +4765,13 @@
       <c r="B53" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="52"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="59"/>
       <c r="J53" s="27" t="s">
         <v>83</v>
       </c>
@@ -4790,13 +4790,13 @@
       <c r="B54" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="52"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="59"/>
       <c r="J54" s="27" t="s">
         <v>83</v>
       </c>
@@ -4815,13 +4815,13 @@
       <c r="B55" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="57"/>
-      <c r="I55" s="52"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="59"/>
       <c r="J55" s="27" t="s">
         <v>83</v>
       </c>
@@ -4838,23 +4838,23 @@
         <v>158</v>
       </c>
       <c r="B56" s="51"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="57"/>
-      <c r="F56" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="I56" s="52"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" s="59"/>
       <c r="J56" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="K56" s="52"/>
+      <c r="K56" s="59"/>
       <c r="L56" s="14"/>
       <c r="M56" s="19" t="s">
         <v>124</v>
@@ -4865,21 +4865,21 @@
         <v>157</v>
       </c>
       <c r="B57" s="51"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57" t="s">
+      <c r="C57" s="58"/>
+      <c r="D57" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="E57" s="57"/>
-      <c r="F57" s="57" t="s">
+      <c r="E57" s="58"/>
+      <c r="F57" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57" t="s">
+      <c r="G57" s="58"/>
+      <c r="H57" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="I57" s="52"/>
+      <c r="I57" s="59"/>
       <c r="J57" s="51"/>
-      <c r="K57" s="52"/>
+      <c r="K57" s="59"/>
       <c r="L57" s="14"/>
       <c r="M57" s="19" t="s">
         <v>159</v>
@@ -4893,26 +4893,26 @@
         <v>84</v>
       </c>
       <c r="C58" s="18"/>
-      <c r="D58" s="57" t="s">
+      <c r="D58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F58" s="57" t="s">
+      <c r="F58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="G58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H58" s="57" t="s">
+      <c r="H58" s="58" t="s">
         <v>84</v>
       </c>
       <c r="I58" s="18" t="s">
         <v>78</v>
       </c>
       <c r="J58" s="51"/>
-      <c r="K58" s="52"/>
+      <c r="K58" s="59"/>
       <c r="L58" s="14"/>
       <c r="M58" s="19" t="s">
         <v>125</v>
@@ -4924,20 +4924,20 @@
       </c>
       <c r="B59" s="51"/>
       <c r="C59" s="18"/>
-      <c r="D59" s="57"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="F59" s="57"/>
+      <c r="F59" s="58"/>
       <c r="G59" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="H59" s="57"/>
+      <c r="H59" s="58"/>
       <c r="I59" s="18" t="s">
         <v>153</v>
       </c>
       <c r="J59" s="51"/>
-      <c r="K59" s="52"/>
+      <c r="K59" s="59"/>
       <c r="L59" s="14"/>
       <c r="M59" s="19" t="s">
         <v>160</v>
@@ -4948,29 +4948,29 @@
         <v>155</v>
       </c>
       <c r="B60" s="27"/>
-      <c r="C60" s="57" t="s">
+      <c r="C60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="57" t="s">
+      <c r="E60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="F60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G60" s="57" t="s">
+      <c r="G60" s="58" t="s">
         <v>84</v>
       </c>
       <c r="H60" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="I60" s="52" t="s">
+      <c r="I60" s="59" t="s">
         <v>84</v>
       </c>
       <c r="J60" s="51"/>
-      <c r="K60" s="52"/>
+      <c r="K60" s="59"/>
       <c r="L60" s="13"/>
       <c r="M60" s="19" t="s">
         <v>126</v>
@@ -4981,69 +4981,69 @@
         <v>162</v>
       </c>
       <c r="B61" s="27"/>
-      <c r="C61" s="59"/>
+      <c r="C61" s="56"/>
       <c r="D61" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="E61" s="59"/>
+      <c r="E61" s="56"/>
       <c r="F61" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="G61" s="59"/>
+      <c r="G61" s="56"/>
       <c r="H61" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="I61" s="54"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="54"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="57"/>
       <c r="L61" s="14"/>
       <c r="M61" s="19" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="63"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="56"/>
-      <c r="J62" s="63"/>
-      <c r="K62" s="56"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="54"/>
       <c r="L62" s="14"/>
     </row>
     <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="53"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="59"/>
-      <c r="I63" s="54"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="54"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="57"/>
       <c r="L63" s="14"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="63"/>
-      <c r="C64" s="55"/>
-      <c r="D64" s="55" t="s">
+      <c r="B64" s="52"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="55"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="55"/>
-      <c r="H64" s="55"/>
-      <c r="I64" s="56"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="53"/>
+      <c r="I64" s="54"/>
       <c r="J64" s="33" t="s">
         <v>81</v>
       </c>
@@ -5065,17 +5065,17 @@
       <c r="B65" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C65" s="57"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="57" t="s">
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G65" s="57"/>
-      <c r="H65" s="57" t="s">
+      <c r="G65" s="58"/>
+      <c r="H65" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I65" s="52"/>
+      <c r="I65" s="59"/>
       <c r="J65" s="18" t="s">
         <v>81</v>
       </c>
@@ -5094,19 +5094,19 @@
       <c r="B66" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="57"/>
-      <c r="F66" s="57" t="s">
+      <c r="C66" s="58"/>
+      <c r="D66" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="57"/>
-      <c r="H66" s="57" t="s">
+      <c r="G66" s="58"/>
+      <c r="H66" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I66" s="52"/>
+      <c r="I66" s="59"/>
       <c r="J66" s="27" t="s">
         <v>81</v>
       </c>
@@ -5125,19 +5125,19 @@
       <c r="B67" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="57"/>
-      <c r="D67" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E67" s="57"/>
-      <c r="F67" s="57" t="s">
+      <c r="C67" s="58"/>
+      <c r="D67" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="58"/>
+      <c r="F67" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G67" s="57"/>
-      <c r="H67" s="57" t="s">
+      <c r="G67" s="58"/>
+      <c r="H67" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="I67" s="52"/>
+      <c r="I67" s="59"/>
       <c r="J67" s="27" t="s">
         <v>81</v>
       </c>
@@ -5177,19 +5177,19 @@
       <c r="B69" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="57"/>
-      <c r="D69" s="57" t="s">
+      <c r="C69" s="58"/>
+      <c r="D69" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="E69" s="57"/>
-      <c r="F69" s="57" t="s">
+      <c r="E69" s="58"/>
+      <c r="F69" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="G69" s="57"/>
-      <c r="H69" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="I69" s="52"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I69" s="59"/>
       <c r="J69" s="27" t="s">
         <v>83</v>
       </c>
@@ -5205,20 +5205,20 @@
       <c r="A70" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="63"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="G70" s="55"/>
-      <c r="H70" s="55"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="55"/>
-      <c r="K70" s="56"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="54"/>
       <c r="L70" s="14"/>
-      <c r="M70" s="58" t="s">
+      <c r="M70" s="66" t="s">
         <v>133</v>
       </c>
     </row>
@@ -5229,15 +5229,15 @@
       <c r="B71" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57" t="s">
+      <c r="C71" s="58"/>
+      <c r="D71" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="52"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="59"/>
       <c r="J71" s="27" t="s">
         <v>140</v>
       </c>
@@ -5245,22 +5245,22 @@
         <v>140</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="58"/>
+      <c r="M71" s="66"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B72" s="51"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="52"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="59"/>
       <c r="J72" s="27"/>
       <c r="K72" s="26"/>
       <c r="L72" s="14"/>
@@ -5273,15 +5273,15 @@
         <v>142</v>
       </c>
       <c r="B73" s="51"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E73" s="57"/>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="57"/>
-      <c r="I73" s="52"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="58"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="59"/>
       <c r="J73" s="27"/>
       <c r="K73" s="26"/>
       <c r="L73" s="14"/>
@@ -5293,18 +5293,18 @@
       <c r="A74" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="53"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="59"/>
-      <c r="E74" s="59"/>
-      <c r="F74" s="59" t="s">
+      <c r="B74" s="55"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G74" s="59"/>
-      <c r="H74" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="I74" s="54"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="I74" s="57"/>
       <c r="J74" s="29" t="s">
         <v>83</v>
       </c>
@@ -5323,19 +5323,19 @@
       <c r="B75" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E75" s="57"/>
-      <c r="F75" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G75" s="57"/>
-      <c r="H75" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="I75" s="52"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I75" s="59"/>
       <c r="J75" s="27" t="s">
         <v>83</v>
       </c>
@@ -5351,22 +5351,22 @@
       <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="C76" s="65"/>
-      <c r="D76" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" s="65"/>
-      <c r="F76" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="G76" s="65"/>
-      <c r="H76" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="I76" s="66"/>
+      <c r="B76" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="I76" s="62"/>
       <c r="J76" s="40" t="s">
         <v>83</v>
       </c>
@@ -5380,6 +5380,106 @@
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="J56:K61"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="M39:M41"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="M70:M71"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J62:K63"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D64:I64"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B62:I63"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:K70"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="B29:I30"/>
     <mergeCell ref="J29:K30"/>
@@ -5404,106 +5504,6 @@
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:K70"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="M70:M71"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="J62:K63"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D64:I64"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B62:I63"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="J56:K61"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H67:I67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>